<commit_message>
Improved table formats and read files and mapping stats
</commit_message>
<xml_diff>
--- a/sample_info/A_rabiei_isolate_list_for_wgs.xlsx
+++ b/sample_info/A_rabiei_isolate_list_for_wgs.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\Ford_Griffith\A_rabiei_genotyping\A_rabiei_WGS\A_rabiei_WGS_analysis\sample_info\"/>
     </mc:Choice>
@@ -19,7 +19,7 @@
     <sheet name="Path_score" sheetId="7" r:id="rId4"/>
     <sheet name="Sheet1" sheetId="1" r:id="rId5"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId6"/>
-    <sheet name="sample_haplotype_details" sheetId="8" r:id="rId7"/>
+    <sheet name="sample_haplotype_details" r:id="rId14" sheetId="8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <fileRecoveryPr repairLoad="1"/>
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1554" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2089" uniqueCount="212">
   <si>
     <t>Isolate</t>
   </si>
@@ -710,6 +710,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2757,17 +2758,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="3" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.7109375" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="11.5703125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13.42578125" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="10.5703125" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="11.140625" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="15.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
+    <col min="2" max="3" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="12.7109375" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="11.5703125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="10.140625" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="13.42578125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="10.5703125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="15.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -4579,10 +4580,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="20.42578125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="43.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="16.0" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="10.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="20.42578125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="43.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -5549,8 +5550,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11" style="69" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="16384" width="9.140625" style="69" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="69" width="11.0" collapsed="true"/>
+    <col min="2" max="16384" style="69" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -5653,18 +5654,18 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" style="24" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="11.42578125" style="24" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="7.140625" style="24" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="13.85546875" style="24" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="9.5703125" style="24" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="12.28515625" style="24" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="9.42578125" style="24" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="8" style="24" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="14" style="28" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.28515625" style="24" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="9.7109375" style="24" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="16384" width="9.140625" style="24" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="24" width="10.28515625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="24" width="11.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="24" width="7.140625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="24" width="13.85546875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="24" width="9.5703125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="24" width="12.28515625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="24" width="9.42578125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="24" width="8.0" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" style="28" width="14.0" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" style="24" width="11.28515625" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" style="24" width="9.7109375" collapsed="true"/>
+    <col min="12" max="16384" style="24" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
@@ -7127,30 +7128,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:O41"/>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:N41"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.42578125" customWidth="1"/>
-    <col min="6" max="6" width="10" customWidth="1"/>
-    <col min="7" max="7" width="13.28515625" customWidth="1"/>
-    <col min="8" max="8" width="10.28515625" customWidth="1"/>
-    <col min="9" max="9" width="0" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="15.28515625" customWidth="1"/>
-    <col min="11" max="11" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="0" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="9.28515625" hidden="1" customWidth="1"/>
-    <col min="14" max="15" width="12.28515625" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -7161,7 +7147,7 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>211</v>
+        <v>116</v>
       </c>
       <c r="E1" t="s">
         <v>83</v>
@@ -7197,27 +7183,27 @@
         <v>200</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2">
       <c r="A2" t="s">
-        <v>89</v>
+        <v>32</v>
       </c>
       <c r="B2" t="s">
-        <v>90</v>
+        <v>50</v>
       </c>
       <c r="C2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2">
-        <v>2017</v>
+        <v>15</v>
+      </c>
+      <c r="D2" t="n">
+        <v>2014.0</v>
       </c>
       <c r="E2" t="s">
-        <v>88</v>
+        <v>21</v>
       </c>
       <c r="F2" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="G2" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="H2" t="s">
         <v>10</v>
@@ -7225,46 +7211,46 @@
       <c r="I2" t="s">
         <v>10</v>
       </c>
-      <c r="J2">
-        <v>5</v>
+      <c r="J2" t="n">
+        <v>1.0</v>
       </c>
       <c r="K2" t="s">
         <v>206</v>
       </c>
       <c r="L2" t="s">
-        <v>209</v>
+        <v>21</v>
       </c>
       <c r="M2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="N2" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="O2" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="3">
       <c r="A3" t="s">
-        <v>91</v>
+        <v>74</v>
       </c>
       <c r="B3" t="s">
-        <v>90</v>
+        <v>51</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3">
-        <v>2017</v>
+        <v>15</v>
+      </c>
+      <c r="D3" t="n">
+        <v>2015.0</v>
       </c>
       <c r="E3" t="s">
-        <v>88</v>
+        <v>3</v>
       </c>
       <c r="F3" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="G3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H3" t="s">
         <v>10</v>
@@ -7272,43 +7258,43 @@
       <c r="I3" t="s">
         <v>10</v>
       </c>
-      <c r="J3">
-        <v>5</v>
+      <c r="J3" t="n">
+        <v>2.0</v>
       </c>
       <c r="K3" t="s">
         <v>206</v>
       </c>
       <c r="L3" t="s">
-        <v>209</v>
+        <v>3</v>
       </c>
       <c r="M3" t="s">
-        <v>193</v>
+        <v>201</v>
       </c>
       <c r="N3" t="s">
-        <v>194</v>
+        <v>201</v>
       </c>
       <c r="O3" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4">
       <c r="A4" t="s">
-        <v>85</v>
+        <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>86</v>
+        <v>51</v>
       </c>
       <c r="C4" t="s">
-        <v>87</v>
-      </c>
-      <c r="D4">
-        <v>2017</v>
+        <v>15</v>
+      </c>
+      <c r="D4" t="n">
+        <v>2015.0</v>
       </c>
       <c r="E4" t="s">
-        <v>88</v>
+        <v>3</v>
       </c>
       <c r="F4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G4" t="s">
         <v>10</v>
@@ -7319,46 +7305,46 @@
       <c r="I4" t="s">
         <v>10</v>
       </c>
-      <c r="J4">
-        <v>5</v>
+      <c r="J4" t="n">
+        <v>4.0</v>
       </c>
       <c r="K4" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="L4" t="s">
-        <v>209</v>
+        <v>3</v>
       </c>
       <c r="M4" t="s">
-        <v>201</v>
+        <v>189</v>
       </c>
       <c r="N4" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="O4" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="5">
       <c r="A5" t="s">
-        <v>84</v>
+        <v>41</v>
       </c>
       <c r="B5" t="s">
-        <v>81</v>
+        <v>51</v>
       </c>
       <c r="C5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5">
-        <v>2017</v>
+        <v>15</v>
+      </c>
+      <c r="D5" t="n">
+        <v>2015.0</v>
       </c>
       <c r="E5" t="s">
         <v>3</v>
       </c>
       <c r="F5" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="G5" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="H5" t="s">
         <v>10</v>
@@ -7366,37 +7352,37 @@
       <c r="I5" t="s">
         <v>10</v>
       </c>
-      <c r="J5">
-        <v>5</v>
+      <c r="J5" t="n">
+        <v>1.0</v>
       </c>
       <c r="K5" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="L5" t="s">
         <v>3</v>
       </c>
       <c r="M5" t="s">
-        <v>201</v>
+        <v>189</v>
       </c>
       <c r="N5" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="O5" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="6">
       <c r="A6" t="s">
-        <v>95</v>
+        <v>17</v>
       </c>
       <c r="B6" t="s">
-        <v>96</v>
+        <v>51</v>
       </c>
       <c r="C6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6">
-        <v>2017</v>
+        <v>15</v>
+      </c>
+      <c r="D6" t="n">
+        <v>2015.0</v>
       </c>
       <c r="E6" t="s">
         <v>3</v>
@@ -7408,98 +7394,98 @@
         <v>10</v>
       </c>
       <c r="H6" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I6" t="s">
         <v>10</v>
       </c>
-      <c r="J6">
-        <v>4</v>
+      <c r="J6" t="n">
+        <v>4.0</v>
       </c>
       <c r="K6" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="L6" t="s">
         <v>3</v>
       </c>
       <c r="M6" t="s">
-        <v>201</v>
+        <v>189</v>
       </c>
       <c r="N6" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="O6" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7">
       <c r="A7" t="s">
-        <v>93</v>
+        <v>35</v>
       </c>
       <c r="B7" t="s">
-        <v>94</v>
+        <v>50</v>
       </c>
       <c r="C7" t="s">
-        <v>87</v>
-      </c>
-      <c r="D7">
-        <v>2017</v>
+        <v>15</v>
+      </c>
+      <c r="D7" t="n">
+        <v>2015.0</v>
       </c>
       <c r="E7" t="s">
-        <v>88</v>
+        <v>3</v>
       </c>
       <c r="F7" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="G7" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="H7" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="I7" t="s">
-        <v>10</v>
-      </c>
-      <c r="J7">
-        <v>4</v>
+        <v>28</v>
+      </c>
+      <c r="J7" t="n">
+        <v>0.0</v>
       </c>
       <c r="K7" t="s">
         <v>206</v>
       </c>
       <c r="L7" t="s">
-        <v>209</v>
+        <v>3</v>
       </c>
       <c r="M7" t="s">
-        <v>201</v>
+        <v>189</v>
       </c>
       <c r="N7" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="O7" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8">
       <c r="A8" t="s">
-        <v>92</v>
+        <v>27</v>
       </c>
       <c r="B8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C8" t="s">
         <v>15</v>
       </c>
-      <c r="D8">
-        <v>2016</v>
+      <c r="D8" t="n">
+        <v>2015.0</v>
       </c>
       <c r="E8" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="F8" t="s">
         <v>9</v>
       </c>
       <c r="G8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H8" t="s">
         <v>10</v>
@@ -7507,28 +7493,28 @@
       <c r="I8" t="s">
         <v>10</v>
       </c>
-      <c r="J8">
-        <v>4</v>
+      <c r="J8" t="n">
+        <v>3.0</v>
       </c>
       <c r="K8" t="s">
         <v>206</v>
       </c>
       <c r="L8" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="M8" t="s">
-        <v>201</v>
+        <v>189</v>
       </c>
       <c r="N8" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="O8" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>99</v>
       </c>
       <c r="B9" t="s">
         <v>51</v>
@@ -7536,17 +7522,17 @@
       <c r="C9" t="s">
         <v>15</v>
       </c>
-      <c r="D9">
-        <v>2015</v>
+      <c r="D9" t="n">
+        <v>2016.0</v>
       </c>
       <c r="E9" t="s">
         <v>3</v>
       </c>
       <c r="F9" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="G9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H9" t="s">
         <v>10</v>
@@ -7554,11 +7540,11 @@
       <c r="I9" t="s">
         <v>10</v>
       </c>
-      <c r="J9">
-        <v>4</v>
+      <c r="J9" t="n">
+        <v>2.0</v>
       </c>
       <c r="K9" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="L9" t="s">
         <v>3</v>
@@ -7567,15 +7553,15 @@
         <v>189</v>
       </c>
       <c r="N9" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="O9" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>75</v>
       </c>
       <c r="B10" t="s">
         <v>51</v>
@@ -7583,8 +7569,8 @@
       <c r="C10" t="s">
         <v>15</v>
       </c>
-      <c r="D10">
-        <v>2015</v>
+      <c r="D10" t="n">
+        <v>2016.0</v>
       </c>
       <c r="E10" t="s">
         <v>3</v>
@@ -7593,7 +7579,7 @@
         <v>9</v>
       </c>
       <c r="G10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H10" t="s">
         <v>10</v>
@@ -7601,11 +7587,11 @@
       <c r="I10" t="s">
         <v>10</v>
       </c>
-      <c r="J10">
-        <v>4</v>
+      <c r="J10" t="n">
+        <v>3.0</v>
       </c>
       <c r="K10" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="L10" t="s">
         <v>3</v>
@@ -7614,27 +7600,27 @@
         <v>189</v>
       </c>
       <c r="N10" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="O10" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11">
       <c r="A11" t="s">
-        <v>22</v>
+        <v>92</v>
       </c>
       <c r="B11" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C11" t="s">
-        <v>13</v>
-      </c>
-      <c r="D11">
-        <v>2014</v>
+        <v>15</v>
+      </c>
+      <c r="D11" t="n">
+        <v>2016.0</v>
       </c>
       <c r="E11" t="s">
-        <v>102</v>
+        <v>3</v>
       </c>
       <c r="F11" t="s">
         <v>9</v>
@@ -7648,37 +7634,37 @@
       <c r="I11" t="s">
         <v>10</v>
       </c>
-      <c r="J11">
-        <v>4</v>
+      <c r="J11" t="n">
+        <v>4.0</v>
       </c>
       <c r="K11" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="L11" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M11" t="s">
-        <v>191</v>
+        <v>201</v>
       </c>
       <c r="N11" t="s">
-        <v>194</v>
+        <v>201</v>
       </c>
       <c r="O11" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12">
       <c r="A12" t="s">
-        <v>47</v>
+        <v>76</v>
       </c>
       <c r="B12" t="s">
-        <v>7</v>
+        <v>51</v>
       </c>
       <c r="C12" t="s">
-        <v>8</v>
-      </c>
-      <c r="D12">
-        <v>2013</v>
+        <v>15</v>
+      </c>
+      <c r="D12" t="n">
+        <v>2016.0</v>
       </c>
       <c r="E12" t="s">
         <v>3</v>
@@ -7687,7 +7673,7 @@
         <v>9</v>
       </c>
       <c r="G12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H12" t="s">
         <v>10</v>
@@ -7695,46 +7681,46 @@
       <c r="I12" t="s">
         <v>10</v>
       </c>
-      <c r="J12">
-        <v>4</v>
+      <c r="J12" t="n">
+        <v>3.0</v>
       </c>
       <c r="K12" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="L12" t="s">
         <v>3</v>
       </c>
       <c r="M12" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="N12" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="O12" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13">
       <c r="A13" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="B13" t="s">
-        <v>90</v>
+        <v>103</v>
       </c>
       <c r="C13" t="s">
-        <v>13</v>
-      </c>
-      <c r="D13">
-        <v>2017</v>
+        <v>15</v>
+      </c>
+      <c r="D13" t="n">
+        <v>2016.0</v>
       </c>
       <c r="E13" t="s">
-        <v>88</v>
+        <v>3</v>
       </c>
       <c r="F13" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="G13" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="H13" t="s">
         <v>10</v>
@@ -7742,46 +7728,46 @@
       <c r="I13" t="s">
         <v>10</v>
       </c>
-      <c r="J13">
-        <v>3</v>
+      <c r="J13" t="n">
+        <v>1.0</v>
       </c>
       <c r="K13" t="s">
         <v>206</v>
       </c>
       <c r="L13" t="s">
-        <v>209</v>
+        <v>3</v>
       </c>
       <c r="M13" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="N13" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="O13" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="14">
       <c r="A14" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="B14" t="s">
-        <v>51</v>
+        <v>103</v>
       </c>
       <c r="C14" t="s">
         <v>15</v>
       </c>
-      <c r="D14">
-        <v>2017</v>
+      <c r="D14" t="n">
+        <v>2016.0</v>
       </c>
       <c r="E14" t="s">
         <v>3</v>
       </c>
       <c r="F14" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="G14" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="H14" t="s">
         <v>10</v>
@@ -7789,8 +7775,8 @@
       <c r="I14" t="s">
         <v>10</v>
       </c>
-      <c r="J14">
-        <v>3</v>
+      <c r="J14" t="n">
+        <v>1.0</v>
       </c>
       <c r="K14" t="s">
         <v>206</v>
@@ -7805,21 +7791,21 @@
         <v>194</v>
       </c>
       <c r="O14" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="15">
       <c r="A15" t="s">
-        <v>97</v>
+        <v>113</v>
       </c>
       <c r="B15" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C15" t="s">
-        <v>8</v>
-      </c>
-      <c r="D15">
-        <v>2016</v>
+        <v>15</v>
+      </c>
+      <c r="D15" t="n">
+        <v>2017.0</v>
       </c>
       <c r="E15" t="s">
         <v>3</v>
@@ -7836,8 +7822,8 @@
       <c r="I15" t="s">
         <v>10</v>
       </c>
-      <c r="J15">
-        <v>3</v>
+      <c r="J15" t="n">
+        <v>3.0</v>
       </c>
       <c r="K15" t="s">
         <v>206</v>
@@ -7846,7 +7832,7 @@
         <v>3</v>
       </c>
       <c r="M15" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="N15" t="s">
         <v>194</v>
@@ -7855,18 +7841,18 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16">
       <c r="A16" t="s">
-        <v>77</v>
+        <v>97</v>
       </c>
       <c r="B16" t="s">
-        <v>81</v>
+        <v>52</v>
       </c>
       <c r="C16" t="s">
         <v>8</v>
       </c>
-      <c r="D16">
-        <v>2016</v>
+      <c r="D16" t="n">
+        <v>2016.0</v>
       </c>
       <c r="E16" t="s">
         <v>3</v>
@@ -7883,8 +7869,8 @@
       <c r="I16" t="s">
         <v>10</v>
       </c>
-      <c r="J16">
-        <v>3</v>
+      <c r="J16" t="n">
+        <v>3.0</v>
       </c>
       <c r="K16" t="s">
         <v>206</v>
@@ -7893,92 +7879,92 @@
         <v>3</v>
       </c>
       <c r="M16" t="s">
+        <v>190</v>
+      </c>
+      <c r="N16" t="s">
+        <v>194</v>
+      </c>
+      <c r="O16" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>77</v>
+      </c>
+      <c r="B17" t="s">
+        <v>81</v>
+      </c>
+      <c r="C17" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" t="n">
+        <v>2016.0</v>
+      </c>
+      <c r="E17" t="s">
+        <v>3</v>
+      </c>
+      <c r="F17" t="s">
+        <v>9</v>
+      </c>
+      <c r="G17" t="s">
+        <v>9</v>
+      </c>
+      <c r="H17" t="s">
+        <v>10</v>
+      </c>
+      <c r="I17" t="s">
+        <v>10</v>
+      </c>
+      <c r="J17" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="K17" t="s">
+        <v>206</v>
+      </c>
+      <c r="L17" t="s">
+        <v>3</v>
+      </c>
+      <c r="M17" t="s">
         <v>201</v>
       </c>
-      <c r="N16" t="s">
+      <c r="N17" t="s">
         <v>201</v>
       </c>
-      <c r="O16" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>75</v>
-      </c>
-      <c r="B17" t="s">
-        <v>51</v>
-      </c>
-      <c r="C17" t="s">
-        <v>15</v>
-      </c>
-      <c r="D17">
-        <v>2016</v>
-      </c>
-      <c r="E17" t="s">
-        <v>3</v>
-      </c>
-      <c r="F17" t="s">
-        <v>9</v>
-      </c>
-      <c r="G17" t="s">
-        <v>9</v>
-      </c>
-      <c r="H17" t="s">
-        <v>10</v>
-      </c>
-      <c r="I17" t="s">
-        <v>10</v>
-      </c>
-      <c r="J17">
-        <v>3</v>
-      </c>
-      <c r="K17" t="s">
-        <v>207</v>
-      </c>
-      <c r="L17" t="s">
-        <v>3</v>
-      </c>
-      <c r="M17" t="s">
-        <v>189</v>
-      </c>
-      <c r="N17" t="s">
-        <v>194</v>
-      </c>
       <c r="O17" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18">
       <c r="A18" t="s">
-        <v>76</v>
+        <v>142</v>
       </c>
       <c r="B18" t="s">
-        <v>51</v>
+        <v>148</v>
       </c>
       <c r="C18" t="s">
-        <v>15</v>
-      </c>
-      <c r="D18">
-        <v>2016</v>
+        <v>8</v>
+      </c>
+      <c r="D18" t="n">
+        <v>2017.0</v>
       </c>
       <c r="E18" t="s">
         <v>3</v>
       </c>
       <c r="F18" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="G18" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="H18" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="I18" t="s">
-        <v>10</v>
-      </c>
-      <c r="J18">
-        <v>3</v>
+        <v>28</v>
+      </c>
+      <c r="J18" t="n">
+        <v>0.0</v>
       </c>
       <c r="K18" t="s">
         <v>206</v>
@@ -7987,27 +7973,27 @@
         <v>3</v>
       </c>
       <c r="M18" t="s">
-        <v>189</v>
+        <v>201</v>
       </c>
       <c r="N18" t="s">
-        <v>194</v>
+        <v>201</v>
       </c>
       <c r="O18" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19">
       <c r="A19" t="s">
-        <v>23</v>
+        <v>95</v>
       </c>
       <c r="B19" t="s">
-        <v>52</v>
+        <v>96</v>
       </c>
       <c r="C19" t="s">
-        <v>8</v>
-      </c>
-      <c r="D19">
-        <v>2015</v>
+        <v>13</v>
+      </c>
+      <c r="D19" t="n">
+        <v>2017.0</v>
       </c>
       <c r="E19" t="s">
         <v>3</v>
@@ -8016,16 +8002,16 @@
         <v>9</v>
       </c>
       <c r="G19" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H19" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I19" t="s">
         <v>10</v>
       </c>
-      <c r="J19">
-        <v>3</v>
+      <c r="J19" t="n">
+        <v>4.0</v>
       </c>
       <c r="K19" t="s">
         <v>206</v>
@@ -8040,39 +8026,39 @@
         <v>201</v>
       </c>
       <c r="O19" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="20">
       <c r="A20" t="s">
-        <v>24</v>
+        <v>107</v>
       </c>
       <c r="B20" t="s">
-        <v>52</v>
+        <v>108</v>
       </c>
       <c r="C20" t="s">
-        <v>8</v>
-      </c>
-      <c r="D20">
-        <v>2015</v>
+        <v>15</v>
+      </c>
+      <c r="D20" t="n">
+        <v>2017.0</v>
       </c>
       <c r="E20" t="s">
         <v>3</v>
       </c>
       <c r="F20" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="G20" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="H20" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="I20" t="s">
-        <v>10</v>
-      </c>
-      <c r="J20">
-        <v>3</v>
+        <v>28</v>
+      </c>
+      <c r="J20" t="n">
+        <v>0.0</v>
       </c>
       <c r="K20" t="s">
         <v>206</v>
@@ -8087,30 +8073,30 @@
         <v>201</v>
       </c>
       <c r="O20" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21">
       <c r="A21" t="s">
-        <v>25</v>
+        <v>84</v>
       </c>
       <c r="B21" t="s">
-        <v>64</v>
+        <v>81</v>
       </c>
       <c r="C21" t="s">
         <v>8</v>
       </c>
-      <c r="D21">
-        <v>2015</v>
+      <c r="D21" t="n">
+        <v>2017.0</v>
       </c>
       <c r="E21" t="s">
         <v>3</v>
       </c>
       <c r="F21" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G21" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H21" t="s">
         <v>10</v>
@@ -8118,8 +8104,8 @@
       <c r="I21" t="s">
         <v>10</v>
       </c>
-      <c r="J21">
-        <v>3</v>
+      <c r="J21" t="n">
+        <v>5.0</v>
       </c>
       <c r="K21" t="s">
         <v>206</v>
@@ -8134,21 +8120,21 @@
         <v>201</v>
       </c>
       <c r="O21" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="22">
       <c r="A22" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="B22" t="s">
-        <v>64</v>
+        <v>7</v>
       </c>
       <c r="C22" t="s">
         <v>8</v>
       </c>
-      <c r="D22">
-        <v>2015</v>
+      <c r="D22" t="n">
+        <v>2013.0</v>
       </c>
       <c r="E22" t="s">
         <v>3</v>
@@ -8157,7 +8143,7 @@
         <v>9</v>
       </c>
       <c r="G22" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H22" t="s">
         <v>10</v>
@@ -8165,37 +8151,37 @@
       <c r="I22" t="s">
         <v>10</v>
       </c>
-      <c r="J22">
-        <v>3</v>
+      <c r="J22" t="n">
+        <v>4.0</v>
       </c>
       <c r="K22" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="L22" t="s">
         <v>3</v>
       </c>
       <c r="M22" t="s">
-        <v>201</v>
+        <v>190</v>
       </c>
       <c r="N22" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="O22" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="23">
       <c r="A23" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="B23" t="s">
-        <v>64</v>
+        <v>7</v>
       </c>
       <c r="C23" t="s">
         <v>8</v>
       </c>
-      <c r="D23">
-        <v>2015</v>
+      <c r="D23" t="n">
+        <v>2013.0</v>
       </c>
       <c r="E23" t="s">
         <v>3</v>
@@ -8212,8 +8198,8 @@
       <c r="I23" t="s">
         <v>10</v>
       </c>
-      <c r="J23">
-        <v>3</v>
+      <c r="J23" t="n">
+        <v>3.0</v>
       </c>
       <c r="K23" t="s">
         <v>206</v>
@@ -8231,24 +8217,24 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24">
       <c r="A24" t="s">
-        <v>27</v>
+        <v>71</v>
       </c>
       <c r="B24" t="s">
-        <v>50</v>
+        <v>7</v>
       </c>
       <c r="C24" t="s">
-        <v>15</v>
-      </c>
-      <c r="D24">
-        <v>2015</v>
+        <v>8</v>
+      </c>
+      <c r="D24" t="n">
+        <v>2013.0</v>
       </c>
       <c r="E24" t="s">
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="F24" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="G24" t="s">
         <v>9</v>
@@ -8259,37 +8245,37 @@
       <c r="I24" t="s">
         <v>10</v>
       </c>
-      <c r="J24">
-        <v>3</v>
+      <c r="J24" t="n">
+        <v>2.0</v>
       </c>
       <c r="K24" t="s">
         <v>206</v>
       </c>
       <c r="L24" t="s">
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="M24" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="N24" t="s">
         <v>194</v>
       </c>
       <c r="O24" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25">
       <c r="A25" t="s">
-        <v>72</v>
+        <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>7</v>
+        <v>52</v>
       </c>
       <c r="C25" t="s">
         <v>8</v>
       </c>
-      <c r="D25">
-        <v>2013</v>
+      <c r="D25" t="n">
+        <v>2015.0</v>
       </c>
       <c r="E25" t="s">
         <v>3</v>
@@ -8306,8 +8292,8 @@
       <c r="I25" t="s">
         <v>10</v>
       </c>
-      <c r="J25">
-        <v>3</v>
+      <c r="J25" t="n">
+        <v>3.0</v>
       </c>
       <c r="K25" t="s">
         <v>206</v>
@@ -8316,33 +8302,33 @@
         <v>3</v>
       </c>
       <c r="M25" t="s">
-        <v>190</v>
+        <v>201</v>
       </c>
       <c r="N25" t="s">
-        <v>194</v>
+        <v>201</v>
       </c>
       <c r="O25" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26">
       <c r="A26" t="s">
-        <v>101</v>
+        <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>106</v>
+        <v>52</v>
       </c>
       <c r="C26" t="s">
-        <v>13</v>
-      </c>
-      <c r="D26">
-        <v>2016</v>
+        <v>8</v>
+      </c>
+      <c r="D26" t="n">
+        <v>2015.0</v>
       </c>
       <c r="E26" t="s">
-        <v>102</v>
+        <v>3</v>
       </c>
       <c r="F26" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="G26" t="s">
         <v>9</v>
@@ -8353,43 +8339,43 @@
       <c r="I26" t="s">
         <v>10</v>
       </c>
-      <c r="J26">
-        <v>2</v>
+      <c r="J26" t="n">
+        <v>3.0</v>
       </c>
       <c r="K26" t="s">
         <v>206</v>
       </c>
       <c r="L26" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M26" t="s">
-        <v>192</v>
+        <v>201</v>
       </c>
       <c r="N26" t="s">
-        <v>194</v>
+        <v>201</v>
       </c>
       <c r="O26" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27">
       <c r="A27" t="s">
-        <v>99</v>
+        <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>51</v>
+        <v>64</v>
       </c>
       <c r="C27" t="s">
-        <v>15</v>
-      </c>
-      <c r="D27">
-        <v>2016</v>
+        <v>8</v>
+      </c>
+      <c r="D27" t="n">
+        <v>2015.0</v>
       </c>
       <c r="E27" t="s">
         <v>3</v>
       </c>
       <c r="F27" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="G27" t="s">
         <v>9</v>
@@ -8400,8 +8386,8 @@
       <c r="I27" t="s">
         <v>10</v>
       </c>
-      <c r="J27">
-        <v>2</v>
+      <c r="J27" t="n">
+        <v>3.0</v>
       </c>
       <c r="K27" t="s">
         <v>206</v>
@@ -8410,33 +8396,33 @@
         <v>3</v>
       </c>
       <c r="M27" t="s">
-        <v>189</v>
+        <v>201</v>
       </c>
       <c r="N27" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="O27" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28">
       <c r="A28" t="s">
-        <v>74</v>
+        <v>38</v>
       </c>
       <c r="B28" t="s">
-        <v>51</v>
+        <v>64</v>
       </c>
       <c r="C28" t="s">
-        <v>15</v>
-      </c>
-      <c r="D28">
-        <v>2015</v>
+        <v>8</v>
+      </c>
+      <c r="D28" t="n">
+        <v>2015.0</v>
       </c>
       <c r="E28" t="s">
         <v>3</v>
       </c>
       <c r="F28" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="G28" t="s">
         <v>9</v>
@@ -8447,8 +8433,8 @@
       <c r="I28" t="s">
         <v>10</v>
       </c>
-      <c r="J28">
-        <v>2</v>
+      <c r="J28" t="n">
+        <v>3.0</v>
       </c>
       <c r="K28" t="s">
         <v>206</v>
@@ -8463,27 +8449,27 @@
         <v>201</v>
       </c>
       <c r="O28" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29">
       <c r="A29" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="B29" t="s">
-        <v>7</v>
+        <v>64</v>
       </c>
       <c r="C29" t="s">
         <v>8</v>
       </c>
-      <c r="D29">
-        <v>2013</v>
+      <c r="D29" t="n">
+        <v>2015.0</v>
       </c>
       <c r="E29" t="s">
         <v>3</v>
       </c>
       <c r="F29" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="G29" t="s">
         <v>9</v>
@@ -8494,8 +8480,8 @@
       <c r="I29" t="s">
         <v>10</v>
       </c>
-      <c r="J29">
-        <v>2</v>
+      <c r="J29" t="n">
+        <v>3.0</v>
       </c>
       <c r="K29" t="s">
         <v>206</v>
@@ -8510,21 +8496,21 @@
         <v>194</v>
       </c>
       <c r="O29" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30">
       <c r="A30" t="s">
-        <v>143</v>
+        <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>145</v>
+        <v>49</v>
       </c>
       <c r="C30" t="s">
         <v>13</v>
       </c>
-      <c r="D30">
-        <v>2016</v>
+      <c r="D30" t="n">
+        <v>2014.0</v>
       </c>
       <c r="E30" t="s">
         <v>102</v>
@@ -8541,40 +8527,40 @@
       <c r="I30" t="s">
         <v>10</v>
       </c>
-      <c r="J30">
-        <v>1</v>
+      <c r="J30" t="n">
+        <v>1.0</v>
       </c>
       <c r="K30" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="L30" t="s">
         <v>4</v>
       </c>
       <c r="M30" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="N30" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="O30" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="31">
       <c r="A31" t="s">
-        <v>104</v>
+        <v>34</v>
       </c>
       <c r="B31" t="s">
-        <v>103</v>
+        <v>49</v>
       </c>
       <c r="C31" t="s">
-        <v>15</v>
-      </c>
-      <c r="D31">
-        <v>2016</v>
+        <v>13</v>
+      </c>
+      <c r="D31" t="n">
+        <v>2014.0</v>
       </c>
       <c r="E31" t="s">
-        <v>3</v>
+        <v>102</v>
       </c>
       <c r="F31" t="s">
         <v>28</v>
@@ -8583,51 +8569,51 @@
         <v>28</v>
       </c>
       <c r="H31" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="I31" t="s">
-        <v>10</v>
-      </c>
-      <c r="J31">
-        <v>1</v>
+        <v>28</v>
+      </c>
+      <c r="J31" t="n">
+        <v>0.0</v>
       </c>
       <c r="K31" t="s">
         <v>206</v>
       </c>
       <c r="L31" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M31" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="N31" t="s">
         <v>194</v>
       </c>
       <c r="O31" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="32">
       <c r="A32" t="s">
-        <v>105</v>
+        <v>22</v>
       </c>
       <c r="B32" t="s">
-        <v>103</v>
+        <v>49</v>
       </c>
       <c r="C32" t="s">
-        <v>15</v>
-      </c>
-      <c r="D32">
-        <v>2016</v>
+        <v>13</v>
+      </c>
+      <c r="D32" t="n">
+        <v>2014.0</v>
       </c>
       <c r="E32" t="s">
-        <v>3</v>
+        <v>102</v>
       </c>
       <c r="F32" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="G32" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
       <c r="H32" t="s">
         <v>10</v>
@@ -8635,46 +8621,46 @@
       <c r="I32" t="s">
         <v>10</v>
       </c>
-      <c r="J32">
-        <v>1</v>
+      <c r="J32" t="n">
+        <v>4.0</v>
       </c>
       <c r="K32" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="L32" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M32" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="N32" t="s">
         <v>194</v>
       </c>
       <c r="O32" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="33">
       <c r="A33" t="s">
-        <v>41</v>
+        <v>101</v>
       </c>
       <c r="B33" t="s">
-        <v>51</v>
+        <v>106</v>
       </c>
       <c r="C33" t="s">
-        <v>15</v>
-      </c>
-      <c r="D33">
-        <v>2015</v>
+        <v>13</v>
+      </c>
+      <c r="D33" t="n">
+        <v>2016.0</v>
       </c>
       <c r="E33" t="s">
-        <v>3</v>
+        <v>102</v>
       </c>
       <c r="F33" t="s">
         <v>28</v>
       </c>
       <c r="G33" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="H33" t="s">
         <v>10</v>
@@ -8682,37 +8668,37 @@
       <c r="I33" t="s">
         <v>10</v>
       </c>
-      <c r="J33">
-        <v>1</v>
+      <c r="J33" t="n">
+        <v>2.0</v>
       </c>
       <c r="K33" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="L33" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M33" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="N33" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="O33" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="34">
       <c r="A34" t="s">
-        <v>29</v>
+        <v>143</v>
       </c>
       <c r="B34" t="s">
-        <v>49</v>
+        <v>145</v>
       </c>
       <c r="C34" t="s">
         <v>13</v>
       </c>
-      <c r="D34">
-        <v>2014</v>
+      <c r="D34" t="n">
+        <v>2016.0</v>
       </c>
       <c r="E34" t="s">
         <v>102</v>
@@ -8729,46 +8715,46 @@
       <c r="I34" t="s">
         <v>10</v>
       </c>
-      <c r="J34">
-        <v>1</v>
+      <c r="J34" t="n">
+        <v>1.0</v>
       </c>
       <c r="K34" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="L34" t="s">
         <v>4</v>
       </c>
       <c r="M34" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="N34" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="O34" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="35">
       <c r="A35" t="s">
-        <v>32</v>
+        <v>85</v>
       </c>
       <c r="B35" t="s">
-        <v>50</v>
+        <v>86</v>
       </c>
       <c r="C35" t="s">
-        <v>15</v>
-      </c>
-      <c r="D35">
-        <v>2014</v>
+        <v>87</v>
+      </c>
+      <c r="D35" t="n">
+        <v>2017.0</v>
       </c>
       <c r="E35" t="s">
-        <v>21</v>
+        <v>88</v>
       </c>
       <c r="F35" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
       <c r="G35" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
       <c r="H35" t="s">
         <v>10</v>
@@ -8776,26 +8762,26 @@
       <c r="I35" t="s">
         <v>10</v>
       </c>
-      <c r="J35">
-        <v>1</v>
+      <c r="J35" t="n">
+        <v>5.0</v>
       </c>
       <c r="K35" t="s">
         <v>206</v>
       </c>
       <c r="L35" t="s">
-        <v>21</v>
+        <v>209</v>
       </c>
       <c r="M35" t="s">
-        <v>189</v>
+        <v>201</v>
       </c>
       <c r="N35" t="s">
-        <v>194</v>
+        <v>201</v>
       </c>
       <c r="O35" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="36">
       <c r="A36" t="s">
         <v>109</v>
       </c>
@@ -8805,8 +8791,8 @@
       <c r="C36" t="s">
         <v>87</v>
       </c>
-      <c r="D36">
-        <v>2017</v>
+      <c r="D36" t="n">
+        <v>2017.0</v>
       </c>
       <c r="E36" t="s">
         <v>88</v>
@@ -8823,8 +8809,8 @@
       <c r="I36" t="s">
         <v>28</v>
       </c>
-      <c r="J36">
-        <v>0</v>
+      <c r="J36" t="n">
+        <v>0.0</v>
       </c>
       <c r="K36" t="s">
         <v>206</v>
@@ -8842,9 +8828,9 @@
         <v>28</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="37">
       <c r="A37" t="s">
-        <v>114</v>
+        <v>93</v>
       </c>
       <c r="B37" t="s">
         <v>94</v>
@@ -8852,26 +8838,26 @@
       <c r="C37" t="s">
         <v>87</v>
       </c>
-      <c r="D37">
-        <v>2017</v>
+      <c r="D37" t="n">
+        <v>2017.0</v>
       </c>
       <c r="E37" t="s">
         <v>88</v>
       </c>
       <c r="F37" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="G37" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
       <c r="H37" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="I37" t="s">
-        <v>28</v>
-      </c>
-      <c r="J37">
-        <v>0</v>
+        <v>10</v>
+      </c>
+      <c r="J37" t="n">
+        <v>4.0</v>
       </c>
       <c r="K37" t="s">
         <v>206</v>
@@ -8886,24 +8872,24 @@
         <v>201</v>
       </c>
       <c r="O37" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="38">
       <c r="A38" t="s">
-        <v>142</v>
+        <v>114</v>
       </c>
       <c r="B38" t="s">
-        <v>148</v>
+        <v>94</v>
       </c>
       <c r="C38" t="s">
-        <v>8</v>
-      </c>
-      <c r="D38">
-        <v>2017</v>
+        <v>87</v>
+      </c>
+      <c r="D38" t="n">
+        <v>2017.0</v>
       </c>
       <c r="E38" t="s">
-        <v>3</v>
+        <v>88</v>
       </c>
       <c r="F38" t="s">
         <v>28</v>
@@ -8917,14 +8903,14 @@
       <c r="I38" t="s">
         <v>28</v>
       </c>
-      <c r="J38">
-        <v>0</v>
+      <c r="J38" t="n">
+        <v>0.0</v>
       </c>
       <c r="K38" t="s">
         <v>206</v>
       </c>
       <c r="L38" t="s">
-        <v>3</v>
+        <v>209</v>
       </c>
       <c r="M38" t="s">
         <v>201</v>
@@ -8936,178 +8922,149 @@
         <v>28</v>
       </c>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="39">
       <c r="A39" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="B39" t="s">
-        <v>108</v>
+        <v>90</v>
       </c>
       <c r="C39" t="s">
-        <v>15</v>
-      </c>
-      <c r="D39">
-        <v>2017</v>
+        <v>13</v>
+      </c>
+      <c r="D39" t="n">
+        <v>2017.0</v>
       </c>
       <c r="E39" t="s">
-        <v>3</v>
+        <v>88</v>
       </c>
       <c r="F39" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="G39" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="H39" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
       <c r="I39" t="s">
-        <v>28</v>
-      </c>
-      <c r="J39">
-        <v>0</v>
+        <v>10</v>
+      </c>
+      <c r="J39" t="n">
+        <v>3.0</v>
       </c>
       <c r="K39" t="s">
         <v>206</v>
       </c>
       <c r="L39" t="s">
-        <v>3</v>
+        <v>209</v>
       </c>
       <c r="M39" t="s">
-        <v>201</v>
+        <v>191</v>
       </c>
       <c r="N39" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="O39" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="40">
       <c r="A40" t="s">
-        <v>35</v>
+        <v>89</v>
       </c>
       <c r="B40" t="s">
-        <v>50</v>
+        <v>90</v>
       </c>
       <c r="C40" t="s">
-        <v>15</v>
-      </c>
-      <c r="D40">
-        <v>2015</v>
+        <v>13</v>
+      </c>
+      <c r="D40" t="n">
+        <v>2017.0</v>
       </c>
       <c r="E40" t="s">
-        <v>3</v>
+        <v>88</v>
       </c>
       <c r="F40" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
       <c r="G40" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
       <c r="H40" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
       <c r="I40" t="s">
-        <v>28</v>
-      </c>
-      <c r="J40">
-        <v>0</v>
+        <v>10</v>
+      </c>
+      <c r="J40" t="n">
+        <v>5.0</v>
       </c>
       <c r="K40" t="s">
         <v>206</v>
       </c>
       <c r="L40" t="s">
-        <v>3</v>
+        <v>209</v>
       </c>
       <c r="M40" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="N40" t="s">
-        <v>194</v>
+        <v>199</v>
       </c>
       <c r="O40" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="41">
       <c r="A41" t="s">
-        <v>34</v>
+        <v>91</v>
       </c>
       <c r="B41" t="s">
-        <v>49</v>
+        <v>90</v>
       </c>
       <c r="C41" t="s">
         <v>13</v>
       </c>
-      <c r="D41">
-        <v>2014</v>
+      <c r="D41" t="n">
+        <v>2017.0</v>
       </c>
       <c r="E41" t="s">
-        <v>102</v>
+        <v>88</v>
       </c>
       <c r="F41" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
       <c r="G41" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
       <c r="H41" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
       <c r="I41" t="s">
-        <v>28</v>
-      </c>
-      <c r="J41">
-        <v>0</v>
+        <v>10</v>
+      </c>
+      <c r="J41" t="n">
+        <v>5.0</v>
       </c>
       <c r="K41" t="s">
         <v>206</v>
       </c>
       <c r="L41" t="s">
-        <v>4</v>
+        <v>209</v>
       </c>
       <c r="M41" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="N41" t="s">
         <v>194</v>
       </c>
       <c r="O41" t="s">
-        <v>28</v>
+        <v>210</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="J2:J41">
-    <cfRule type="colorScale" priority="5">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F2:H41">
-    <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
-      <formula>"High"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
-      <formula>"Medium"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
-      <formula>"Moderate"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
-      <formula>"Low"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Manual fix of isolate list Excel file
</commit_message>
<xml_diff>
--- a/sample_info/A_rabiei_isolate_list_for_wgs.xlsx
+++ b/sample_info/A_rabiei_isolate_list_for_wgs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Ford_Griffith\A_rabiei_genotyping\A_rabiei_WGS\A_rabiei_WGS_analysis\sample_info\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://griffitheduau-my.sharepoint.com/personal/i_bar_griffith_edu_au/Documents/Research/A_rabiei/Sophie_A_rabiei_WGS/A_rabiei_WGS_analysis/sample_info/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:20001_{25A96603-2CF4-4541-A4EE-BBBA829B6F9E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{E453E0E2-A4C1-422F-8FE4-5E27F853EFC5}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="52845" yWindow="9900" windowWidth="21600" windowHeight="11145" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sequenced" sheetId="3" r:id="rId1"/>
@@ -47,7 +47,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>soeadmin:</t>
         </r>
@@ -56,7 +56,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 This was contaminated with bacterial DNA and was not included in the WGS analysis</t>
@@ -749,14 +749,14 @@
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
@@ -1212,97 +1212,7 @@
     <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
     <cellStyle name="Normal 3" xfId="2" xr:uid="{1570D574-0313-47FF-B72D-FD18F6F46147}"/>
   </cellStyles>
-  <dxfs count="46">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="40">
     <dxf>
       <font>
         <strike val="0"/>
@@ -1696,6 +1606,36 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -2384,41 +2324,41 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D5572FCD-A755-4762-8393-7A04F393885C}" name="Table2" displayName="Table2" ref="A1:L41" totalsRowShown="0" headerRowDxfId="45" dataDxfId="43" headerRowBorderDxfId="44" tableBorderDxfId="42">
-  <sortState ref="A2:L41">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D5572FCD-A755-4762-8393-7A04F393885C}" name="Table2" displayName="Table2" ref="A1:L41" totalsRowShown="0" headerRowDxfId="39" dataDxfId="37" headerRowBorderDxfId="38" tableBorderDxfId="36">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L41">
     <sortCondition descending="1" ref="J2:J41"/>
     <sortCondition ref="D2:D41"/>
     <sortCondition ref="C2:C41"/>
   </sortState>
   <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{B4D2A589-505E-4080-B340-A922F5551E86}" name="Isolate" dataDxfId="41"/>
-    <tableColumn id="2" xr3:uid="{1E8522FF-47CB-41CB-AEC2-04139993991D}" name="Site" dataDxfId="40"/>
-    <tableColumn id="3" xr3:uid="{74F0F75E-3122-43B0-92CD-B7DA10E13882}" name="State" dataDxfId="39"/>
+    <tableColumn id="1" xr3:uid="{B4D2A589-505E-4080-B340-A922F5551E86}" name="Isolate" dataDxfId="35"/>
+    <tableColumn id="2" xr3:uid="{1E8522FF-47CB-41CB-AEC2-04139993991D}" name="Site" dataDxfId="34"/>
+    <tableColumn id="3" xr3:uid="{74F0F75E-3122-43B0-92CD-B7DA10E13882}" name="State" dataDxfId="33"/>
     <tableColumn id="12" xr3:uid="{9F84C422-8790-42EE-8A7B-89FD537EF716}" name="Sequenced"/>
-    <tableColumn id="4" xr3:uid="{17413865-617C-4ED1-BDF1-5C2B05C22F0F}" name="Collection_Year" dataDxfId="38"/>
-    <tableColumn id="5" xr3:uid="{24DF00BE-59E7-4115-AA74-162DE658E041}" name="Host Cultivar" dataDxfId="37"/>
-    <tableColumn id="6" xr3:uid="{09C5A796-9CA2-4C3F-9CA4-4F214BCE9523}" name="ICC3996" dataDxfId="36"/>
-    <tableColumn id="7" xr3:uid="{D0D03B17-F57C-4DB1-BB40-36D57EC88EF4}" name="Genesis090" dataDxfId="35"/>
-    <tableColumn id="8" xr3:uid="{F4C28E67-F4E7-4D2B-B545-79507B6DC0B2}" name="HatTrick" dataDxfId="34"/>
-    <tableColumn id="9" xr3:uid="{9D7E32AB-0701-4980-97FF-69E517E2B623}" name="Rating" dataDxfId="33"/>
-    <tableColumn id="10" xr3:uid="{E7D666DB-F408-411A-8E5F-6DF06B0A97FB}" name="Pathogenicity" dataDxfId="32"/>
-    <tableColumn id="11" xr3:uid="{7C84594C-4BF0-4263-8CFF-59E09782F30F}" name="Haplotype" dataDxfId="31"/>
+    <tableColumn id="4" xr3:uid="{17413865-617C-4ED1-BDF1-5C2B05C22F0F}" name="Collection_Year" dataDxfId="32"/>
+    <tableColumn id="5" xr3:uid="{24DF00BE-59E7-4115-AA74-162DE658E041}" name="Host Cultivar" dataDxfId="31"/>
+    <tableColumn id="6" xr3:uid="{09C5A796-9CA2-4C3F-9CA4-4F214BCE9523}" name="ICC3996" dataDxfId="30"/>
+    <tableColumn id="7" xr3:uid="{D0D03B17-F57C-4DB1-BB40-36D57EC88EF4}" name="Genesis090" dataDxfId="29"/>
+    <tableColumn id="8" xr3:uid="{F4C28E67-F4E7-4D2B-B545-79507B6DC0B2}" name="HatTrick" dataDxfId="28"/>
+    <tableColumn id="9" xr3:uid="{9D7E32AB-0701-4980-97FF-69E517E2B623}" name="Rating" dataDxfId="27"/>
+    <tableColumn id="10" xr3:uid="{E7D666DB-F408-411A-8E5F-6DF06B0A97FB}" name="Pathogenicity" dataDxfId="26"/>
+    <tableColumn id="11" xr3:uid="{7C84594C-4BF0-4263-8CFF-59E09782F30F}" name="Haplotype" dataDxfId="25"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{AA5A7274-40DF-49DD-96EA-F8EDB374FA68}" name="Table3" displayName="Table3" ref="A1:D64" totalsRowShown="0" headerRowBorderDxfId="30" tableBorderDxfId="29" totalsRowBorderDxfId="28">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{AA5A7274-40DF-49DD-96EA-F8EDB374FA68}" name="Table3" displayName="Table3" ref="A1:D64" totalsRowShown="0" headerRowBorderDxfId="24" tableBorderDxfId="23" totalsRowBorderDxfId="22">
   <autoFilter ref="A1:D64" xr:uid="{DD96D66A-74A9-40FD-9BD1-BA6D4E069ABC}"/>
-  <sortState ref="A10:D64">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A10:D64">
     <sortCondition ref="C1:C64"/>
   </sortState>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{9D327445-B8AD-408B-860C-D230AF620F2A}" name="Submission_id" dataDxfId="27"/>
-    <tableColumn id="2" xr3:uid="{C68FDDA2-6D6D-46A4-9F4C-8AEF287AFCC3}" name="Isolate" dataDxfId="26"/>
-    <tableColumn id="3" xr3:uid="{358560ED-8842-4D42-B41E-D83DF3F9D166}" name="Sequencing_Centre" dataDxfId="25"/>
-    <tableColumn id="4" xr3:uid="{A846A1E7-9119-449E-B626-201497999850}" name="Comments" dataDxfId="24"/>
+    <tableColumn id="1" xr3:uid="{9D327445-B8AD-408B-860C-D230AF620F2A}" name="Submission_id" dataDxfId="21"/>
+    <tableColumn id="2" xr3:uid="{C68FDDA2-6D6D-46A4-9F4C-8AEF287AFCC3}" name="Isolate" dataDxfId="20"/>
+    <tableColumn id="3" xr3:uid="{358560ED-8842-4D42-B41E-D83DF3F9D166}" name="Sequencing_Centre" dataDxfId="19"/>
+    <tableColumn id="4" xr3:uid="{A846A1E7-9119-449E-B626-201497999850}" name="Comments" dataDxfId="18"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2426,7 +2366,7 @@
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{21EE8601-D93F-4E1D-89BA-AD90D26868FA}" name="Table4" displayName="Table4" ref="A1:O41" totalsRowShown="0">
-  <sortState ref="A2:O41">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:O41">
     <sortCondition descending="1" ref="J2:J41"/>
     <sortCondition descending="1" ref="D2:D41"/>
     <sortCondition ref="C2:C41"/>
@@ -2453,23 +2393,23 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:K33" totalsRowShown="0" headerRowDxfId="23" dataDxfId="21" headerRowBorderDxfId="22" tableBorderDxfId="20">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:K33" totalsRowShown="0" headerRowDxfId="14" dataDxfId="12" headerRowBorderDxfId="13" tableBorderDxfId="11">
   <autoFilter ref="A1:K33" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <sortState ref="A2:K33">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K33">
     <sortCondition ref="A1:A33"/>
   </sortState>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Isolate" dataDxfId="19"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Site" dataDxfId="18"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="State" dataDxfId="17"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Host_Cultivar" dataDxfId="16"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="ICC3996" dataDxfId="15"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Genesis090" dataDxfId="14"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="HatTrick" dataDxfId="13"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Rating" dataDxfId="12"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Pathogenicity" dataDxfId="11"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Haplotype" dataDxfId="10"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Sequenced" dataDxfId="9"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Isolate" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Site" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="State" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Host_Cultivar" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="ICC3996" dataDxfId="6"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Genesis090" dataDxfId="5"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="HatTrick" dataDxfId="4"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Rating" dataDxfId="3"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Pathogenicity" dataDxfId="2"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Haplotype" dataDxfId="1"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Sequenced" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2802,22 +2742,22 @@
       <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="3" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.7109375" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="11.5703125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13.42578125" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="10.5703125" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="11.140625" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="15.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="10.59765625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="3" width="13.1328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.73046875" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="12.265625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="11.59765625" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="10.1328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="11.1328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="13.3984375" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="10.59765625" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="11.1328125" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="15.265625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A1" s="41" t="s">
         <v>0</v>
       </c>
@@ -2855,7 +2795,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A2" s="48" t="s">
         <v>47</v>
       </c>
@@ -2893,7 +2833,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A3" s="48" t="s">
         <v>22</v>
       </c>
@@ -2931,7 +2871,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A4" s="48" t="s">
         <v>14</v>
       </c>
@@ -2969,7 +2909,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A5" s="48" t="s">
         <v>17</v>
       </c>
@@ -3007,7 +2947,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A6" s="49" t="s">
         <v>92</v>
       </c>
@@ -3043,7 +2983,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A7" s="48" t="s">
         <v>89</v>
       </c>
@@ -3079,7 +3019,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A8" s="49" t="s">
         <v>91</v>
       </c>
@@ -3115,7 +3055,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A9" s="49" t="s">
         <v>85</v>
       </c>
@@ -3151,7 +3091,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A10" s="49" t="s">
         <v>84</v>
       </c>
@@ -3187,7 +3127,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A11" s="49" t="s">
         <v>72</v>
       </c>
@@ -3225,7 +3165,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A12" s="49" t="s">
         <v>23</v>
       </c>
@@ -3263,7 +3203,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A13" s="48" t="s">
         <v>24</v>
       </c>
@@ -3301,7 +3241,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A14" s="49" t="s">
         <v>25</v>
       </c>
@@ -3339,7 +3279,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A15" s="48" t="s">
         <v>38</v>
       </c>
@@ -3377,7 +3317,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A16" s="49" t="s">
         <v>78</v>
       </c>
@@ -3415,7 +3355,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A17" s="48" t="s">
         <v>27</v>
       </c>
@@ -3453,7 +3393,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A18" s="49" t="s">
         <v>97</v>
       </c>
@@ -3489,7 +3429,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A19" s="48" t="s">
         <v>77</v>
       </c>
@@ -3525,7 +3465,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A20" s="49" t="s">
         <v>75</v>
       </c>
@@ -3563,7 +3503,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A21" s="48" t="s">
         <v>76</v>
       </c>
@@ -3601,7 +3541,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A22" s="49" t="s">
         <v>95</v>
       </c>
@@ -3637,7 +3577,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A23" s="49" t="s">
         <v>98</v>
       </c>
@@ -3673,7 +3613,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A24" s="49" t="s">
         <v>93</v>
       </c>
@@ -3709,7 +3649,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A25" s="48" t="s">
         <v>113</v>
       </c>
@@ -3745,7 +3685,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A26" s="48" t="s">
         <v>71</v>
       </c>
@@ -3783,7 +3723,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A27" s="49" t="s">
         <v>74</v>
       </c>
@@ -3821,7 +3761,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A28" s="48" t="s">
         <v>101</v>
       </c>
@@ -3859,7 +3799,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A29" s="48" t="s">
         <v>99</v>
       </c>
@@ -3897,7 +3837,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A30" s="48" t="s">
         <v>29</v>
       </c>
@@ -3935,7 +3875,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A31" s="48" t="s">
         <v>32</v>
       </c>
@@ -3973,7 +3913,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A32" s="49" t="s">
         <v>41</v>
       </c>
@@ -4011,7 +3951,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A33" s="49" t="s">
         <v>143</v>
       </c>
@@ -4047,7 +3987,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A34" s="48" t="s">
         <v>104</v>
       </c>
@@ -4085,7 +4025,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A35" s="49" t="s">
         <v>105</v>
       </c>
@@ -4123,7 +4063,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A36" s="49" t="s">
         <v>34</v>
       </c>
@@ -4161,7 +4101,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A37" s="49" t="s">
         <v>35</v>
       </c>
@@ -4199,7 +4139,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A38" s="48" t="s">
         <v>109</v>
       </c>
@@ -4235,7 +4175,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A39" s="48" t="s">
         <v>114</v>
       </c>
@@ -4271,7 +4211,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A40" s="49" t="s">
         <v>142</v>
       </c>
@@ -4307,7 +4247,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A41" s="14" t="s">
         <v>107</v>
       </c>
@@ -4624,15 +4564,15 @@
       <selection activeCell="A44" sqref="A44:D44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="20.42578125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="43.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="10.1328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="20.3984375" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="43.86328125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" s="41" t="s">
         <v>117</v>
       </c>
@@ -4646,7 +4586,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" s="52" t="s">
         <v>32</v>
       </c>
@@ -4658,7 +4598,7 @@
       </c>
       <c r="D2" s="52"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" s="50" t="s">
         <v>74</v>
       </c>
@@ -4670,7 +4610,7 @@
       </c>
       <c r="D3" s="50"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4" s="52" t="s">
         <v>14</v>
       </c>
@@ -4682,7 +4622,7 @@
       </c>
       <c r="D4" s="52"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A5" s="50" t="s">
         <v>118</v>
       </c>
@@ -4696,7 +4636,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A6" s="52" t="s">
         <v>17</v>
       </c>
@@ -4710,7 +4650,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A7" s="50" t="s">
         <v>123</v>
       </c>
@@ -4722,7 +4662,7 @@
       </c>
       <c r="D7" s="50"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A8" s="52" t="s">
         <v>27</v>
       </c>
@@ -4734,7 +4674,7 @@
       </c>
       <c r="D8" s="52"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A9" s="50" t="s">
         <v>124</v>
       </c>
@@ -4748,7 +4688,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A10" s="52" t="s">
         <v>186</v>
       </c>
@@ -4760,7 +4700,7 @@
       </c>
       <c r="D10" s="52"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A11" s="50" t="s">
         <v>75</v>
       </c>
@@ -4772,7 +4712,7 @@
       </c>
       <c r="D11" s="50"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A12" s="52" t="s">
         <v>125</v>
       </c>
@@ -4786,7 +4726,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A13" s="50" t="s">
         <v>174</v>
       </c>
@@ -4798,7 +4738,7 @@
       </c>
       <c r="D13" s="50"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A14" s="52" t="s">
         <v>175</v>
       </c>
@@ -4812,7 +4752,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A15" s="50" t="s">
         <v>76</v>
       </c>
@@ -4824,7 +4764,7 @@
       </c>
       <c r="D15" s="50"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A16" s="52" t="s">
         <v>126</v>
       </c>
@@ -4836,7 +4776,7 @@
       </c>
       <c r="D16" s="52"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A17" s="50" t="s">
         <v>176</v>
       </c>
@@ -4848,7 +4788,7 @@
       </c>
       <c r="D17" s="50"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A18" s="52" t="s">
         <v>127</v>
       </c>
@@ -4860,7 +4800,7 @@
       </c>
       <c r="D18" s="52"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A19" s="50" t="s">
         <v>177</v>
       </c>
@@ -4872,7 +4812,7 @@
       </c>
       <c r="D19" s="50"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A20" s="52" t="s">
         <v>128</v>
       </c>
@@ -4886,7 +4826,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A21" s="50" t="s">
         <v>178</v>
       </c>
@@ -4900,7 +4840,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A22" s="52" t="s">
         <v>179</v>
       </c>
@@ -4914,7 +4854,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A23" s="50" t="s">
         <v>129</v>
       </c>
@@ -4926,7 +4866,7 @@
       </c>
       <c r="D23" s="50"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A24" s="52" t="s">
         <v>180</v>
       </c>
@@ -4938,7 +4878,7 @@
       </c>
       <c r="D24" s="52"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A25" s="50" t="s">
         <v>130</v>
       </c>
@@ -4950,7 +4890,7 @@
       </c>
       <c r="D25" s="50"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A26" s="52" t="s">
         <v>181</v>
       </c>
@@ -4962,7 +4902,7 @@
       </c>
       <c r="D26" s="52"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A27" s="50" t="s">
         <v>77</v>
       </c>
@@ -4974,7 +4914,7 @@
       </c>
       <c r="D27" s="50"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A28" s="52" t="s">
         <v>182</v>
       </c>
@@ -4986,7 +4926,7 @@
       </c>
       <c r="D28" s="52"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A29" s="50" t="s">
         <v>131</v>
       </c>
@@ -4998,7 +4938,7 @@
       </c>
       <c r="D29" s="50"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A30" s="52" t="s">
         <v>183</v>
       </c>
@@ -5010,7 +4950,7 @@
       </c>
       <c r="D30" s="52"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A31" s="50" t="s">
         <v>132</v>
       </c>
@@ -5022,7 +4962,7 @@
       </c>
       <c r="D31" s="50"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A32" s="52" t="s">
         <v>161</v>
       </c>
@@ -5034,7 +4974,7 @@
       </c>
       <c r="D32" s="52"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A33" s="50" t="s">
         <v>133</v>
       </c>
@@ -5046,7 +4986,7 @@
       </c>
       <c r="D33" s="50"/>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A34" s="52" t="s">
         <v>162</v>
       </c>
@@ -5058,7 +4998,7 @@
       </c>
       <c r="D34" s="52"/>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A35" s="50" t="s">
         <v>163</v>
       </c>
@@ -5070,7 +5010,7 @@
       </c>
       <c r="D35" s="50"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A36" s="52" t="s">
         <v>164</v>
       </c>
@@ -5084,7 +5024,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A37" s="50" t="s">
         <v>47</v>
       </c>
@@ -5096,7 +5036,7 @@
       </c>
       <c r="D37" s="50"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A38" s="52" t="s">
         <v>72</v>
       </c>
@@ -5108,7 +5048,7 @@
       </c>
       <c r="D38" s="52"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A39" s="50" t="s">
         <v>71</v>
       </c>
@@ -5120,7 +5060,7 @@
       </c>
       <c r="D39" s="50"/>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A40" s="52" t="s">
         <v>122</v>
       </c>
@@ -5134,7 +5074,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A41" s="50" t="s">
         <v>121</v>
       </c>
@@ -5146,7 +5086,7 @@
       </c>
       <c r="D41" s="50"/>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A42" s="52" t="s">
         <v>119</v>
       </c>
@@ -5158,7 +5098,7 @@
       </c>
       <c r="D42" s="52"/>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A43" s="50" t="s">
         <v>120</v>
       </c>
@@ -5170,7 +5110,7 @@
       </c>
       <c r="D43" s="50"/>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A44" s="52" t="s">
         <v>78</v>
       </c>
@@ -5182,7 +5122,7 @@
       </c>
       <c r="D44" s="52"/>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A45" s="50" t="s">
         <v>29</v>
       </c>
@@ -5194,7 +5134,7 @@
       </c>
       <c r="D45" s="50"/>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A46" s="52" t="s">
         <v>34</v>
       </c>
@@ -5206,7 +5146,7 @@
       </c>
       <c r="D46" s="52"/>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A47" s="50" t="s">
         <v>22</v>
       </c>
@@ -5218,7 +5158,7 @@
       </c>
       <c r="D47" s="50"/>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A48" s="52" t="s">
         <v>134</v>
       </c>
@@ -5232,7 +5172,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A49" s="50" t="s">
         <v>165</v>
       </c>
@@ -5246,7 +5186,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A50" s="52" t="s">
         <v>166</v>
       </c>
@@ -5258,7 +5198,7 @@
       </c>
       <c r="D50" s="52"/>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A51" s="50" t="s">
         <v>135</v>
       </c>
@@ -5272,7 +5212,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A52" s="52" t="s">
         <v>167</v>
       </c>
@@ -5286,7 +5226,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A53" s="50" t="s">
         <v>136</v>
       </c>
@@ -5298,7 +5238,7 @@
       </c>
       <c r="D53" s="50"/>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A54" s="52" t="s">
         <v>168</v>
       </c>
@@ -5310,7 +5250,7 @@
       </c>
       <c r="D54" s="52"/>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A55" s="50" t="s">
         <v>137</v>
       </c>
@@ -5324,7 +5264,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A56" s="52" t="s">
         <v>169</v>
       </c>
@@ -5338,7 +5278,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A57" s="50" t="s">
         <v>138</v>
       </c>
@@ -5350,7 +5290,7 @@
       </c>
       <c r="D57" s="50"/>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A58" s="52" t="s">
         <v>170</v>
       </c>
@@ -5362,7 +5302,7 @@
       </c>
       <c r="D58" s="52"/>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A59" s="50" t="s">
         <v>139</v>
       </c>
@@ -5376,7 +5316,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A60" s="52" t="s">
         <v>171</v>
       </c>
@@ -5390,7 +5330,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A61" s="50" t="s">
         <v>140</v>
       </c>
@@ -5404,7 +5344,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A62" s="52" t="s">
         <v>172</v>
       </c>
@@ -5418,7 +5358,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A63" s="50" t="s">
         <v>141</v>
       </c>
@@ -5432,7 +5372,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A64" s="52" t="s">
         <v>173</v>
       </c>
@@ -5462,9 +5402,9 @@
       <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A1" s="60" t="s">
         <v>117</v>
       </c>
@@ -5505,7 +5445,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A2" s="34">
         <v>8</v>
       </c>
@@ -5528,7 +5468,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A3" s="33">
         <v>13</v>
       </c>
@@ -5594,22 +5534,22 @@
       <selection sqref="A1:O41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.140625" customWidth="1"/>
-    <col min="5" max="5" width="14.42578125" customWidth="1"/>
+    <col min="1" max="1" width="10.1328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.86328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.1328125" customWidth="1"/>
+    <col min="5" max="5" width="14.3984375" customWidth="1"/>
     <col min="6" max="6" width="10" customWidth="1"/>
-    <col min="7" max="7" width="13.28515625" customWidth="1"/>
-    <col min="8" max="8" width="10.28515625" customWidth="1"/>
-    <col min="10" max="10" width="15.28515625" customWidth="1"/>
-    <col min="11" max="11" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.28515625" customWidth="1"/>
-    <col min="14" max="15" width="12.28515625" customWidth="1"/>
+    <col min="7" max="7" width="13.265625" customWidth="1"/>
+    <col min="8" max="8" width="10.265625" customWidth="1"/>
+    <col min="10" max="10" width="15.265625" customWidth="1"/>
+    <col min="11" max="11" width="15.265625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.265625" customWidth="1"/>
+    <col min="14" max="15" width="12.265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5656,7 +5596,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>89</v>
       </c>
@@ -5703,7 +5643,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>91</v>
       </c>
@@ -5750,7 +5690,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>85</v>
       </c>
@@ -5797,7 +5737,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>84</v>
       </c>
@@ -5844,7 +5784,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>95</v>
       </c>
@@ -5891,7 +5831,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>93</v>
       </c>
@@ -5938,7 +5878,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>92</v>
       </c>
@@ -5985,7 +5925,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -6032,7 +5972,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="10" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" hidden="1" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -6079,7 +6019,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>22</v>
       </c>
@@ -6126,7 +6066,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>47</v>
       </c>
@@ -6173,7 +6113,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>98</v>
       </c>
@@ -6220,7 +6160,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>113</v>
       </c>
@@ -6267,7 +6207,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>97</v>
       </c>
@@ -6314,7 +6254,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>77</v>
       </c>
@@ -6361,7 +6301,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>75</v>
       </c>
@@ -6408,7 +6348,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>76</v>
       </c>
@@ -6455,7 +6395,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>23</v>
       </c>
@@ -6502,7 +6442,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>24</v>
       </c>
@@ -6549,7 +6489,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>25</v>
       </c>
@@ -6596,7 +6536,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>38</v>
       </c>
@@ -6643,7 +6583,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>78</v>
       </c>
@@ -6690,7 +6630,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>27</v>
       </c>
@@ -6737,7 +6677,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>72</v>
       </c>
@@ -6784,7 +6724,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>101</v>
       </c>
@@ -6831,7 +6771,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>99</v>
       </c>
@@ -6878,7 +6818,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>74</v>
       </c>
@@ -6925,7 +6865,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>71</v>
       </c>
@@ -6972,7 +6912,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>143</v>
       </c>
@@ -7019,7 +6959,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
         <v>104</v>
       </c>
@@ -7066,7 +7006,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
         <v>105</v>
       </c>
@@ -7113,7 +7053,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
         <v>41</v>
       </c>
@@ -7160,7 +7100,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
         <v>29</v>
       </c>
@@ -7207,7 +7147,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
         <v>32</v>
       </c>
@@ -7254,7 +7194,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
         <v>109</v>
       </c>
@@ -7301,7 +7241,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
         <v>114</v>
       </c>
@@ -7348,7 +7288,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
         <v>142</v>
       </c>
@@ -7395,7 +7335,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
         <v>107</v>
       </c>
@@ -7442,7 +7382,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
         <v>35</v>
       </c>
@@ -7489,7 +7429,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
         <v>34</v>
       </c>
@@ -7538,13 +7478,13 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="F2:I41">
-    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="Low">
+    <cfRule type="containsText" dxfId="17" priority="4" operator="containsText" text="Low">
       <formula>NOT(ISERROR(SEARCH("Low",F2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="3" operator="containsText" text="Moderate">
+    <cfRule type="containsText" dxfId="16" priority="3" operator="containsText" text="Moderate">
       <formula>NOT(ISERROR(SEARCH("Moderate",F2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="2" operator="containsText" text="High">
+    <cfRule type="containsText" dxfId="15" priority="2" operator="containsText" text="High">
       <formula>NOT(ISERROR(SEARCH("High",F2)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7575,13 +7515,13 @@
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="11" style="65" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="16384" width="9.140625" style="65" collapsed="1"/>
+    <col min="2" max="16384" width="9.1328125" style="65" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" s="65" t="s">
         <v>202</v>
       </c>
@@ -7598,7 +7538,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2" s="65" t="s">
         <v>2</v>
       </c>
@@ -7615,7 +7555,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A3" s="65" t="s">
         <v>3</v>
       </c>
@@ -7632,7 +7572,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A4" s="65" t="s">
         <v>4</v>
       </c>
@@ -7649,7 +7589,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A5" s="65" t="s">
         <v>209</v>
       </c>
@@ -7679,23 +7619,23 @@
       <selection activeCell="H35" sqref="H35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" style="24" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="11.42578125" style="24" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="7.140625" style="24" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="13.85546875" style="24" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="9.5703125" style="24" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="12.28515625" style="24" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="9.42578125" style="24" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="10.265625" style="24" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.3984375" style="24" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="7.1328125" style="24" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="13.86328125" style="24" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="9.59765625" style="24" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="12.265625" style="24" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="9.3984375" style="24" customWidth="1" collapsed="1"/>
     <col min="8" max="8" width="8" style="24" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="9" max="9" width="14" style="28" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.28515625" style="24" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="9.7109375" style="24" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="16384" width="9.140625" style="24" collapsed="1"/>
+    <col min="10" max="10" width="11.265625" style="24" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="9.73046875" style="24" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="16384" width="9.1328125" style="24" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -7730,7 +7670,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A2" s="14" t="s">
         <v>32</v>
       </c>
@@ -7765,7 +7705,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A3" s="12" t="s">
         <v>30</v>
       </c>
@@ -7796,7 +7736,7 @@
       <c r="J3" s="12"/>
       <c r="K3" s="8"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A4" s="12" t="s">
         <v>74</v>
       </c>
@@ -7831,7 +7771,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A5" s="14" t="s">
         <v>14</v>
       </c>
@@ -7866,7 +7806,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A6" s="14" t="s">
         <v>41</v>
       </c>
@@ -7901,7 +7841,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A7" s="12" t="s">
         <v>17</v>
       </c>
@@ -7936,7 +7876,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A8" s="14" t="s">
         <v>35</v>
       </c>
@@ -7971,7 +7911,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A9" s="12" t="s">
         <v>27</v>
       </c>
@@ -8006,7 +7946,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A10" s="14" t="s">
         <v>20</v>
       </c>
@@ -8039,7 +7979,7 @@
       </c>
       <c r="K10" s="8"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A11" s="14" t="s">
         <v>75</v>
       </c>
@@ -8074,7 +8014,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A12" s="12" t="s">
         <v>76</v>
       </c>
@@ -8109,7 +8049,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A13" s="14" t="s">
         <v>77</v>
       </c>
@@ -8142,7 +8082,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A14" s="12" t="s">
         <v>48</v>
       </c>
@@ -8175,7 +8115,7 @@
       </c>
       <c r="K14" s="8"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A15" s="12" t="s">
         <v>47</v>
       </c>
@@ -8210,7 +8150,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A16" s="14" t="s">
         <v>72</v>
       </c>
@@ -8245,7 +8185,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A17" s="12" t="s">
         <v>71</v>
       </c>
@@ -8280,7 +8220,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A18" s="14" t="s">
         <v>58</v>
       </c>
@@ -8311,7 +8251,7 @@
       <c r="J18" s="8"/>
       <c r="K18" s="8"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A19" s="12" t="s">
         <v>37</v>
       </c>
@@ -8342,7 +8282,7 @@
       <c r="J19" s="8"/>
       <c r="K19" s="8"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A20" s="12" t="s">
         <v>36</v>
       </c>
@@ -8377,7 +8317,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A21" s="14" t="s">
         <v>60</v>
       </c>
@@ -8408,7 +8348,7 @@
       <c r="J21" s="8"/>
       <c r="K21" s="8"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A22" s="14" t="s">
         <v>23</v>
       </c>
@@ -8443,7 +8383,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A23" s="12" t="s">
         <v>19</v>
       </c>
@@ -8476,7 +8416,7 @@
       </c>
       <c r="K23" s="8"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A24" s="12" t="s">
         <v>24</v>
       </c>
@@ -8511,7 +8451,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A25" s="14" t="s">
         <v>25</v>
       </c>
@@ -8546,7 +8486,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A26" s="12" t="s">
         <v>38</v>
       </c>
@@ -8581,7 +8521,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A27" s="14" t="s">
         <v>78</v>
       </c>
@@ -8616,7 +8556,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A28" s="12" t="s">
         <v>29</v>
       </c>
@@ -8651,7 +8591,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A29" s="14" t="s">
         <v>34</v>
       </c>
@@ -8686,7 +8626,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A30" s="14" t="s">
         <v>12</v>
       </c>
@@ -8719,7 +8659,7 @@
       </c>
       <c r="K30" s="23"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A31" s="12" t="s">
         <v>22</v>
       </c>
@@ -8754,7 +8694,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A32" s="12" t="s">
         <v>33</v>
       </c>
@@ -8787,7 +8727,7 @@
       </c>
       <c r="K32" s="23"/>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A33" s="14" t="s">
         <v>61</v>
       </c>
@@ -8819,7 +8759,7 @@
       <c r="K33" s="23"/>
     </row>
   </sheetData>
-  <sortState ref="M2:M10">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="M2:M10">
     <sortCondition ref="M2"/>
   </sortState>
   <conditionalFormatting sqref="I2:I3 I24:I33 I12:I22 I5:I10">
@@ -8887,14 +8827,14 @@
       <selection sqref="A1:C27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" s="3" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -8905,7 +8845,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>48</v>
       </c>
@@ -8916,7 +8856,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>47</v>
       </c>
@@ -8927,7 +8867,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
         <v>46</v>
       </c>
@@ -8938,12 +8878,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
@@ -8954,7 +8894,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
         <v>22</v>
       </c>
@@ -8965,7 +8905,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
         <v>45</v>
       </c>
@@ -8976,12 +8916,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="s">
         <v>20</v>
       </c>
@@ -8992,7 +8932,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="s">
         <v>44</v>
       </c>
@@ -9003,7 +8943,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A13" s="1" t="s">
         <v>43</v>
       </c>
@@ -9014,7 +8954,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A14" s="1" t="s">
         <v>42</v>
       </c>
@@ -9025,12 +8965,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
@@ -9041,7 +8981,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A17" s="1" t="s">
         <v>17</v>
       </c>
@@ -9052,7 +8992,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A18" s="1" t="s">
         <v>41</v>
       </c>
@@ -9063,7 +9003,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A19" s="1" t="s">
         <v>40</v>
       </c>
@@ -9074,12 +9014,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A21" s="1" t="s">
         <v>39</v>
       </c>
@@ -9090,7 +9030,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A22" s="1" t="s">
         <v>19</v>
       </c>
@@ -9101,7 +9041,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A23" s="1" t="s">
         <v>24</v>
       </c>
@@ -9112,12 +9052,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A25" s="1" t="s">
         <v>25</v>
       </c>
@@ -9128,7 +9068,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A26" s="1" t="s">
         <v>38</v>
       </c>
@@ -9139,7 +9079,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A27" s="1" t="s">
         <v>37</v>
       </c>
@@ -9156,20 +9096,44 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100CF58540B94450B45B7164CDCEF97F187" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="5d8dbd669b9ca3a74eb8709c213c647d">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="6cc093d9-4f30-445e-9010-d0117c74656d" xmlns:ns3="ff1451eb-1820-42ab-a257-e0e71c4d4e64" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="da50ea4e48985e64f93d7c2a3a9e6ff7" ns2:_="" ns3:_="">
-    <xsd:import namespace="6cc093d9-4f30-445e-9010-d0117c74656d"/>
-    <xsd:import namespace="ff1451eb-1820-42ab-a257-e0e71c4d4e64"/>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010038EC5152544FA941B2FCF6FC911C1211" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c0a7b694108ffeb4d5e14fa8f2f5e4a2">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="f38ef60c-44b8-4b3e-b84e-3f774f47ec01" xmlns:ns4="77420ce7-ad61-40a5-b28d-42d2f2a680a0" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7cc2d357fdf517c32b7ae6696f0078b7" ns3:_="" ns4:_="">
+    <xsd:import namespace="f38ef60c-44b8-4b3e-b84e-3f774f47ec01"/>
+    <xsd:import namespace="77420ce7-ad61-40a5-b28d-42d2f2a680a0"/>
     <xsd:element name="properties">
       <xsd:complexType>
         <xsd:sequence>
           <xsd:element name="documentManagement">
             <xsd:complexType>
               <xsd:all>
-                <xsd:element ref="ns2:SharedWithUsers" minOccurs="0"/>
-                <xsd:element ref="ns2:SharedWithDetails" minOccurs="0"/>
                 <xsd:element ref="ns3:MediaServiceMetadata" minOccurs="0"/>
                 <xsd:element ref="ns3:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns4:SharedWithUsers" minOccurs="0"/>
+                <xsd:element ref="ns4:SharedWithDetails" minOccurs="0"/>
+                <xsd:element ref="ns4:SharingHintHash" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceAutoTags" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceLocation" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceAutoKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceKeyPoints" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -9177,10 +9141,68 @@
       </xsd:complexType>
     </xsd:element>
   </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="6cc093d9-4f30-445e-9010-d0117c74656d" elementFormDefault="qualified">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="f38ef60c-44b8-4b3e-b84e-3f774f47ec01" elementFormDefault="qualified">
     <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="SharedWithUsers" ma:index="8" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
+    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="13" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoTags" ma:index="14" nillable="true" ma:displayName="Tags" ma:internalName="MediaServiceAutoTags" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="15" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="16" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="17" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceLocation" ma:index="18" nillable="true" ma:displayName="Location" ma:internalName="MediaServiceLocation" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoKeyPoints" ma:index="19" nillable="true" ma:displayName="MediaServiceAutoKeyPoints" ma:hidden="true" ma:internalName="MediaServiceAutoKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceKeyPoints" ma:index="20" nillable="true" ma:displayName="KeyPoints" ma:internalName="MediaServiceKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="77420ce7-ad61-40a5-b28d-42d2f2a680a0" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="SharedWithUsers" ma:index="10" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
       <xsd:complexType>
         <xsd:complexContent>
           <xsd:extension base="dms:UserMulti">
@@ -9199,25 +9221,16 @@
         </xsd:complexContent>
       </xsd:complexType>
     </xsd:element>
-    <xsd:element name="SharedWithDetails" ma:index="9" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
+    <xsd:element name="SharedWithDetails" ma:index="11" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Note">
           <xsd:maxLength value="255"/>
         </xsd:restriction>
       </xsd:simpleType>
     </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="ff1451eb-1820-42ab-a257-e0e71c4d4e64" elementFormDefault="qualified">
-    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="MediaServiceMetadata" ma:index="10" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+    <xsd:element name="SharingHintHash" ma:index="12" nillable="true" ma:displayName="Sharing Hint Hash" ma:hidden="true" ma:internalName="SharingHintHash" ma:readOnly="true">
       <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceFastMetadata" ma:index="11" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
+        <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
     </xsd:element>
   </xsd:schema>
@@ -9320,36 +9333,19 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5C6D9C8C-AED0-4DD1-A485-921CF3EA82DE}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7AB5AB63-4FEC-4580-8B0C-E2F5F38CD9AC}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="77420ce7-ad61-40a5-b28d-42d2f2a680a0"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="6cc093d9-4f30-445e-9010-d0117c74656d"/>
-    <ds:schemaRef ds:uri="ff1451eb-1820-42ab-a257-e0e71c4d4e64"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="f38ef60c-44b8-4b3e-b84e-3f774f47ec01"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -9363,18 +9359,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7AB5AB63-4FEC-4580-8B0C-E2F5F38CD9AC}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5E51EC21-F22B-490E-8776-BB08FE496BF5}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="6cc093d9-4f30-445e-9010-d0117c74656d"/>
+    <ds:schemaRef ds:uri="f38ef60c-44b8-4b3e-b84e-3f774f47ec01"/>
+    <ds:schemaRef ds:uri="77420ce7-ad61-40a5-b28d-42d2f2a680a0"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="ff1451eb-1820-42ab-a257-e0e71c4d4e64"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updated to use Pacman and Util.R from gist
</commit_message>
<xml_diff>
--- a/sample_info/A_rabiei_isolate_list_for_wgs.xlsx
+++ b/sample_info/A_rabiei_isolate_list_for_wgs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://griffitheduau-my.sharepoint.com/personal/i_bar_griffith_edu_au/Documents/Research/A_rabiei/Sophie_A_rabiei_WGS/A_rabiei_WGS_analysis/sample_info/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{E453E0E2-A4C1-422F-8FE4-5E27F853EFC5}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:20001_{81A9BED5-B4FC-4B70-BACC-F3DD7F67022C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="52845" yWindow="9900" windowWidth="21600" windowHeight="11145" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="13096" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sequenced" sheetId="3" r:id="rId1"/>
@@ -2366,10 +2366,9 @@
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{21EE8601-D93F-4E1D-89BA-AD90D26868FA}" name="Table4" displayName="Table4" ref="A1:O41" totalsRowShown="0">
+  <autoFilter ref="A1:O41" xr:uid="{A72BE80D-98B9-4748-8A02-BE5E4D36E5E1}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:O41">
-    <sortCondition descending="1" ref="J2:J41"/>
-    <sortCondition descending="1" ref="D2:D41"/>
-    <sortCondition ref="C2:C41"/>
+    <sortCondition ref="A2"/>
   </sortState>
   <tableColumns count="15">
     <tableColumn id="1" xr3:uid="{65335CB5-4BCE-4F9D-BEE4-CFCDBFFC4F13}" name="Isolate"/>
@@ -5530,8 +5529,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:O41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection sqref="A1:O41"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:O41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -5598,25 +5597,25 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>89</v>
+        <v>32</v>
       </c>
       <c r="B2" t="s">
-        <v>90</v>
+        <v>50</v>
       </c>
       <c r="C2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D2">
-        <v>2017</v>
+        <v>2014</v>
       </c>
       <c r="E2" t="s">
-        <v>88</v>
+        <v>21</v>
       </c>
       <c r="F2" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="G2" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="H2" t="s">
         <v>10</v>
@@ -5625,45 +5624,45 @@
         <v>10</v>
       </c>
       <c r="J2">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="K2" t="s">
         <v>206</v>
       </c>
       <c r="L2" t="s">
-        <v>209</v>
+        <v>21</v>
       </c>
       <c r="M2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="N2" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="O2" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>91</v>
+        <v>74</v>
       </c>
       <c r="B3" t="s">
-        <v>90</v>
+        <v>51</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D3">
-        <v>2017</v>
+        <v>2015</v>
       </c>
       <c r="E3" t="s">
-        <v>88</v>
+        <v>3</v>
       </c>
       <c r="F3" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="G3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H3" t="s">
         <v>10</v>
@@ -5672,42 +5671,42 @@
         <v>10</v>
       </c>
       <c r="J3">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="K3" t="s">
         <v>206</v>
       </c>
       <c r="L3" t="s">
-        <v>209</v>
+        <v>3</v>
       </c>
       <c r="M3" t="s">
-        <v>193</v>
+        <v>201</v>
       </c>
       <c r="N3" t="s">
-        <v>194</v>
+        <v>201</v>
       </c>
       <c r="O3" t="s">
-        <v>210</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>85</v>
+        <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>86</v>
+        <v>51</v>
       </c>
       <c r="C4" t="s">
-        <v>87</v>
+        <v>15</v>
       </c>
       <c r="D4">
-        <v>2017</v>
+        <v>2015</v>
       </c>
       <c r="E4" t="s">
-        <v>88</v>
+        <v>3</v>
       </c>
       <c r="F4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G4" t="s">
         <v>10</v>
@@ -5719,45 +5718,45 @@
         <v>10</v>
       </c>
       <c r="J4">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K4" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="L4" t="s">
-        <v>209</v>
+        <v>3</v>
       </c>
       <c r="M4" t="s">
-        <v>201</v>
+        <v>189</v>
       </c>
       <c r="N4" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="O4" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>84</v>
+        <v>41</v>
       </c>
       <c r="B5" t="s">
-        <v>81</v>
+        <v>51</v>
       </c>
       <c r="C5" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="D5">
-        <v>2017</v>
+        <v>2015</v>
       </c>
       <c r="E5" t="s">
         <v>3</v>
       </c>
       <c r="F5" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="G5" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="H5" t="s">
         <v>10</v>
@@ -5766,54 +5765,54 @@
         <v>10</v>
       </c>
       <c r="J5">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="K5" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="L5" t="s">
         <v>3</v>
       </c>
       <c r="M5" t="s">
-        <v>201</v>
+        <v>189</v>
       </c>
       <c r="N5" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="O5" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>95</v>
+        <v>35</v>
       </c>
       <c r="B6" t="s">
-        <v>96</v>
+        <v>50</v>
       </c>
       <c r="C6" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D6">
-        <v>2017</v>
+        <v>2015</v>
       </c>
       <c r="E6" t="s">
         <v>3</v>
       </c>
       <c r="F6" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="G6" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="H6" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="I6" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="J6">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="K6" t="s">
         <v>206</v>
@@ -5822,65 +5821,65 @@
         <v>3</v>
       </c>
       <c r="M6" t="s">
-        <v>201</v>
+        <v>189</v>
       </c>
       <c r="N6" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="O6" t="s">
-        <v>204</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>93</v>
+        <v>27</v>
       </c>
       <c r="B7" t="s">
-        <v>94</v>
+        <v>50</v>
       </c>
       <c r="C7" t="s">
-        <v>87</v>
+        <v>15</v>
       </c>
       <c r="D7">
-        <v>2017</v>
+        <v>2015</v>
       </c>
       <c r="E7" t="s">
-        <v>88</v>
+        <v>21</v>
       </c>
       <c r="F7" t="s">
         <v>9</v>
       </c>
       <c r="G7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H7" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I7" t="s">
         <v>10</v>
       </c>
       <c r="J7">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K7" t="s">
         <v>206</v>
       </c>
       <c r="L7" t="s">
-        <v>209</v>
+        <v>21</v>
       </c>
       <c r="M7" t="s">
-        <v>201</v>
+        <v>189</v>
       </c>
       <c r="N7" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="O7" t="s">
-        <v>204</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>92</v>
+        <v>99</v>
       </c>
       <c r="B8" t="s">
         <v>51</v>
@@ -5895,10 +5894,10 @@
         <v>3</v>
       </c>
       <c r="F8" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="G8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H8" t="s">
         <v>10</v>
@@ -5907,7 +5906,7 @@
         <v>10</v>
       </c>
       <c r="J8">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="K8" t="s">
         <v>206</v>
@@ -5916,18 +5915,18 @@
         <v>3</v>
       </c>
       <c r="M8" t="s">
-        <v>201</v>
+        <v>189</v>
       </c>
       <c r="N8" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="O8" t="s">
-        <v>204</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>75</v>
       </c>
       <c r="B9" t="s">
         <v>51</v>
@@ -5936,7 +5935,7 @@
         <v>15</v>
       </c>
       <c r="D9">
-        <v>2015</v>
+        <v>2016</v>
       </c>
       <c r="E9" t="s">
         <v>3</v>
@@ -5945,7 +5944,7 @@
         <v>9</v>
       </c>
       <c r="G9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H9" t="s">
         <v>10</v>
@@ -5954,7 +5953,7 @@
         <v>10</v>
       </c>
       <c r="J9">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K9" t="s">
         <v>207</v>
@@ -5966,10 +5965,10 @@
         <v>189</v>
       </c>
       <c r="N9" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="O9" t="s">
-        <v>204</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:15" hidden="1" x14ac:dyDescent="0.45">
@@ -6021,19 +6020,19 @@
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>22</v>
+        <v>92</v>
       </c>
       <c r="B11" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C11" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D11">
-        <v>2014</v>
+        <v>2016</v>
       </c>
       <c r="E11" t="s">
-        <v>102</v>
+        <v>3</v>
       </c>
       <c r="F11" t="s">
         <v>9</v>
@@ -6051,16 +6050,16 @@
         <v>4</v>
       </c>
       <c r="K11" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="L11" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M11" t="s">
-        <v>191</v>
+        <v>201</v>
       </c>
       <c r="N11" t="s">
-        <v>194</v>
+        <v>201</v>
       </c>
       <c r="O11" t="s">
         <v>204</v>
@@ -6068,16 +6067,16 @@
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>47</v>
+        <v>76</v>
       </c>
       <c r="B12" t="s">
-        <v>7</v>
+        <v>51</v>
       </c>
       <c r="C12" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="D12">
-        <v>2013</v>
+        <v>2016</v>
       </c>
       <c r="E12" t="s">
         <v>3</v>
@@ -6086,7 +6085,7 @@
         <v>9</v>
       </c>
       <c r="G12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H12" t="s">
         <v>10</v>
@@ -6095,45 +6094,45 @@
         <v>10</v>
       </c>
       <c r="J12">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K12" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="L12" t="s">
         <v>3</v>
       </c>
       <c r="M12" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="N12" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="O12" t="s">
-        <v>204</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="B13" t="s">
-        <v>90</v>
+        <v>103</v>
       </c>
       <c r="C13" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D13">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="E13" t="s">
-        <v>88</v>
+        <v>3</v>
       </c>
       <c r="F13" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="G13" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="H13" t="s">
         <v>10</v>
@@ -6142,45 +6141,45 @@
         <v>10</v>
       </c>
       <c r="J13">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K13" t="s">
         <v>206</v>
       </c>
       <c r="L13" t="s">
-        <v>209</v>
+        <v>3</v>
       </c>
       <c r="M13" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="N13" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="O13" t="s">
-        <v>10</v>
+        <v>203</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="B14" t="s">
-        <v>51</v>
+        <v>103</v>
       </c>
       <c r="C14" t="s">
         <v>15</v>
       </c>
       <c r="D14">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="E14" t="s">
         <v>3</v>
       </c>
       <c r="F14" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="G14" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="H14" t="s">
         <v>10</v>
@@ -6189,7 +6188,7 @@
         <v>10</v>
       </c>
       <c r="J14">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K14" t="s">
         <v>206</v>
@@ -6204,21 +6203,21 @@
         <v>194</v>
       </c>
       <c r="O14" t="s">
-        <v>10</v>
+        <v>203</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>97</v>
+        <v>113</v>
       </c>
       <c r="B15" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C15" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="D15">
-        <v>2016</v>
+        <v>2017</v>
       </c>
       <c r="E15" t="s">
         <v>3</v>
@@ -6245,7 +6244,7 @@
         <v>3</v>
       </c>
       <c r="M15" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="N15" t="s">
         <v>194</v>
@@ -6256,10 +6255,10 @@
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>77</v>
+        <v>97</v>
       </c>
       <c r="B16" t="s">
-        <v>81</v>
+        <v>52</v>
       </c>
       <c r="C16" t="s">
         <v>8</v>
@@ -6292,10 +6291,10 @@
         <v>3</v>
       </c>
       <c r="M16" t="s">
-        <v>201</v>
+        <v>190</v>
       </c>
       <c r="N16" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="O16" t="s">
         <v>10</v>
@@ -6303,13 +6302,13 @@
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B17" t="s">
-        <v>51</v>
+        <v>81</v>
       </c>
       <c r="C17" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="D17">
         <v>2016</v>
@@ -6333,16 +6332,16 @@
         <v>3</v>
       </c>
       <c r="K17" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="L17" t="s">
         <v>3</v>
       </c>
       <c r="M17" t="s">
-        <v>189</v>
+        <v>201</v>
       </c>
       <c r="N17" t="s">
-        <v>194</v>
+        <v>201</v>
       </c>
       <c r="O17" t="s">
         <v>10</v>
@@ -6350,34 +6349,34 @@
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
-        <v>76</v>
+        <v>142</v>
       </c>
       <c r="B18" t="s">
-        <v>51</v>
+        <v>148</v>
       </c>
       <c r="C18" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="D18">
-        <v>2016</v>
+        <v>2017</v>
       </c>
       <c r="E18" t="s">
         <v>3</v>
       </c>
       <c r="F18" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="G18" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="H18" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="I18" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="J18">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="K18" t="s">
         <v>206</v>
@@ -6386,27 +6385,27 @@
         <v>3</v>
       </c>
       <c r="M18" t="s">
-        <v>189</v>
+        <v>201</v>
       </c>
       <c r="N18" t="s">
-        <v>194</v>
+        <v>201</v>
       </c>
       <c r="O18" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
-        <v>23</v>
+        <v>95</v>
       </c>
       <c r="B19" t="s">
-        <v>52</v>
+        <v>96</v>
       </c>
       <c r="C19" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D19">
-        <v>2015</v>
+        <v>2017</v>
       </c>
       <c r="E19" t="s">
         <v>3</v>
@@ -6415,16 +6414,16 @@
         <v>9</v>
       </c>
       <c r="G19" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H19" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I19" t="s">
         <v>10</v>
       </c>
       <c r="J19">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K19" t="s">
         <v>206</v>
@@ -6439,39 +6438,39 @@
         <v>201</v>
       </c>
       <c r="O19" t="s">
-        <v>10</v>
+        <v>204</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
-        <v>24</v>
+        <v>107</v>
       </c>
       <c r="B20" t="s">
-        <v>52</v>
+        <v>108</v>
       </c>
       <c r="C20" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="D20">
-        <v>2015</v>
+        <v>2017</v>
       </c>
       <c r="E20" t="s">
         <v>3</v>
       </c>
       <c r="F20" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="G20" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="H20" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="I20" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="J20">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="K20" t="s">
         <v>206</v>
@@ -6486,30 +6485,30 @@
         <v>201</v>
       </c>
       <c r="O20" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
-        <v>25</v>
+        <v>84</v>
       </c>
       <c r="B21" t="s">
-        <v>64</v>
+        <v>81</v>
       </c>
       <c r="C21" t="s">
         <v>8</v>
       </c>
       <c r="D21">
-        <v>2015</v>
+        <v>2017</v>
       </c>
       <c r="E21" t="s">
         <v>3</v>
       </c>
       <c r="F21" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G21" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H21" t="s">
         <v>10</v>
@@ -6518,7 +6517,7 @@
         <v>10</v>
       </c>
       <c r="J21">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="K21" t="s">
         <v>206</v>
@@ -6533,21 +6532,21 @@
         <v>201</v>
       </c>
       <c r="O21" t="s">
-        <v>10</v>
+        <v>210</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="B22" t="s">
-        <v>64</v>
+        <v>7</v>
       </c>
       <c r="C22" t="s">
         <v>8</v>
       </c>
       <c r="D22">
-        <v>2015</v>
+        <v>2013</v>
       </c>
       <c r="E22" t="s">
         <v>3</v>
@@ -6556,7 +6555,7 @@
         <v>9</v>
       </c>
       <c r="G22" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H22" t="s">
         <v>10</v>
@@ -6565,36 +6564,36 @@
         <v>10</v>
       </c>
       <c r="J22">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K22" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="L22" t="s">
         <v>3</v>
       </c>
       <c r="M22" t="s">
-        <v>201</v>
+        <v>190</v>
       </c>
       <c r="N22" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="O22" t="s">
-        <v>10</v>
+        <v>204</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="B23" t="s">
-        <v>64</v>
+        <v>7</v>
       </c>
       <c r="C23" t="s">
         <v>8</v>
       </c>
       <c r="D23">
-        <v>2015</v>
+        <v>2013</v>
       </c>
       <c r="E23" t="s">
         <v>3</v>
@@ -6632,22 +6631,22 @@
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
-        <v>27</v>
+        <v>71</v>
       </c>
       <c r="B24" t="s">
-        <v>50</v>
+        <v>7</v>
       </c>
       <c r="C24" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="D24">
-        <v>2015</v>
+        <v>2013</v>
       </c>
       <c r="E24" t="s">
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="F24" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="G24" t="s">
         <v>9</v>
@@ -6659,36 +6658,36 @@
         <v>10</v>
       </c>
       <c r="J24">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K24" t="s">
         <v>206</v>
       </c>
       <c r="L24" t="s">
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="M24" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="N24" t="s">
         <v>194</v>
       </c>
       <c r="O24" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
-        <v>72</v>
+        <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>7</v>
+        <v>52</v>
       </c>
       <c r="C25" t="s">
         <v>8</v>
       </c>
       <c r="D25">
-        <v>2013</v>
+        <v>2015</v>
       </c>
       <c r="E25" t="s">
         <v>3</v>
@@ -6715,10 +6714,10 @@
         <v>3</v>
       </c>
       <c r="M25" t="s">
-        <v>190</v>
+        <v>201</v>
       </c>
       <c r="N25" t="s">
-        <v>194</v>
+        <v>201</v>
       </c>
       <c r="O25" t="s">
         <v>10</v>
@@ -6726,22 +6725,22 @@
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
-        <v>101</v>
+        <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>106</v>
+        <v>52</v>
       </c>
       <c r="C26" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D26">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="E26" t="s">
-        <v>102</v>
+        <v>3</v>
       </c>
       <c r="F26" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="G26" t="s">
         <v>9</v>
@@ -6753,42 +6752,42 @@
         <v>10</v>
       </c>
       <c r="J26">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K26" t="s">
         <v>206</v>
       </c>
       <c r="L26" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M26" t="s">
-        <v>192</v>
+        <v>201</v>
       </c>
       <c r="N26" t="s">
-        <v>194</v>
+        <v>201</v>
       </c>
       <c r="O26" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
-        <v>99</v>
+        <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>51</v>
+        <v>64</v>
       </c>
       <c r="C27" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="D27">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="E27" t="s">
         <v>3</v>
       </c>
       <c r="F27" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="G27" t="s">
         <v>9</v>
@@ -6800,7 +6799,7 @@
         <v>10</v>
       </c>
       <c r="J27">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K27" t="s">
         <v>206</v>
@@ -6809,24 +6808,24 @@
         <v>3</v>
       </c>
       <c r="M27" t="s">
-        <v>189</v>
+        <v>201</v>
       </c>
       <c r="N27" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="O27" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
-        <v>74</v>
+        <v>38</v>
       </c>
       <c r="B28" t="s">
-        <v>51</v>
+        <v>64</v>
       </c>
       <c r="C28" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="D28">
         <v>2015</v>
@@ -6835,7 +6834,7 @@
         <v>3</v>
       </c>
       <c r="F28" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="G28" t="s">
         <v>9</v>
@@ -6847,7 +6846,7 @@
         <v>10</v>
       </c>
       <c r="J28">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K28" t="s">
         <v>206</v>
@@ -6862,27 +6861,27 @@
         <v>201</v>
       </c>
       <c r="O28" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="B29" t="s">
-        <v>7</v>
+        <v>64</v>
       </c>
       <c r="C29" t="s">
         <v>8</v>
       </c>
       <c r="D29">
-        <v>2013</v>
+        <v>2015</v>
       </c>
       <c r="E29" t="s">
         <v>3</v>
       </c>
       <c r="F29" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="G29" t="s">
         <v>9</v>
@@ -6894,7 +6893,7 @@
         <v>10</v>
       </c>
       <c r="J29">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K29" t="s">
         <v>206</v>
@@ -6909,21 +6908,21 @@
         <v>194</v>
       </c>
       <c r="O29" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
-        <v>143</v>
+        <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>145</v>
+        <v>49</v>
       </c>
       <c r="C30" t="s">
         <v>13</v>
       </c>
       <c r="D30">
-        <v>2016</v>
+        <v>2014</v>
       </c>
       <c r="E30" t="s">
         <v>102</v>
@@ -6944,16 +6943,16 @@
         <v>1</v>
       </c>
       <c r="K30" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="L30" t="s">
         <v>4</v>
       </c>
       <c r="M30" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="N30" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="O30" t="s">
         <v>203</v>
@@ -6961,19 +6960,19 @@
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
-        <v>104</v>
+        <v>34</v>
       </c>
       <c r="B31" t="s">
-        <v>103</v>
+        <v>49</v>
       </c>
       <c r="C31" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D31">
-        <v>2016</v>
+        <v>2014</v>
       </c>
       <c r="E31" t="s">
-        <v>3</v>
+        <v>102</v>
       </c>
       <c r="F31" t="s">
         <v>28</v>
@@ -6982,51 +6981,51 @@
         <v>28</v>
       </c>
       <c r="H31" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="I31" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="J31">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K31" t="s">
         <v>206</v>
       </c>
       <c r="L31" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M31" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="N31" t="s">
         <v>194</v>
       </c>
       <c r="O31" t="s">
-        <v>203</v>
+        <v>28</v>
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
-        <v>105</v>
+        <v>22</v>
       </c>
       <c r="B32" t="s">
-        <v>103</v>
+        <v>49</v>
       </c>
       <c r="C32" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D32">
-        <v>2016</v>
+        <v>2014</v>
       </c>
       <c r="E32" t="s">
-        <v>3</v>
+        <v>102</v>
       </c>
       <c r="F32" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="G32" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
       <c r="H32" t="s">
         <v>10</v>
@@ -7035,45 +7034,45 @@
         <v>10</v>
       </c>
       <c r="J32">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="K32" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="L32" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M32" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="N32" t="s">
         <v>194</v>
       </c>
       <c r="O32" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
-        <v>41</v>
+        <v>101</v>
       </c>
       <c r="B33" t="s">
-        <v>51</v>
+        <v>106</v>
       </c>
       <c r="C33" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D33">
-        <v>2015</v>
+        <v>2016</v>
       </c>
       <c r="E33" t="s">
-        <v>3</v>
+        <v>102</v>
       </c>
       <c r="F33" t="s">
         <v>28</v>
       </c>
       <c r="G33" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="H33" t="s">
         <v>10</v>
@@ -7082,36 +7081,36 @@
         <v>10</v>
       </c>
       <c r="J33">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K33" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="L33" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M33" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="N33" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="O33" t="s">
-        <v>203</v>
+        <v>9</v>
       </c>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
-        <v>29</v>
+        <v>143</v>
       </c>
       <c r="B34" t="s">
-        <v>49</v>
+        <v>145</v>
       </c>
       <c r="C34" t="s">
         <v>13</v>
       </c>
       <c r="D34">
-        <v>2014</v>
+        <v>2016</v>
       </c>
       <c r="E34" t="s">
         <v>102</v>
@@ -7132,16 +7131,16 @@
         <v>1</v>
       </c>
       <c r="K34" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="L34" t="s">
         <v>4</v>
       </c>
       <c r="M34" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="N34" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="O34" t="s">
         <v>203</v>
@@ -7149,25 +7148,25 @@
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
-        <v>32</v>
+        <v>85</v>
       </c>
       <c r="B35" t="s">
-        <v>50</v>
+        <v>86</v>
       </c>
       <c r="C35" t="s">
-        <v>15</v>
+        <v>87</v>
       </c>
       <c r="D35">
-        <v>2014</v>
+        <v>2017</v>
       </c>
       <c r="E35" t="s">
-        <v>21</v>
+        <v>88</v>
       </c>
       <c r="F35" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
       <c r="G35" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
       <c r="H35" t="s">
         <v>10</v>
@@ -7176,22 +7175,22 @@
         <v>10</v>
       </c>
       <c r="J35">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="K35" t="s">
         <v>206</v>
       </c>
       <c r="L35" t="s">
-        <v>21</v>
+        <v>209</v>
       </c>
       <c r="M35" t="s">
-        <v>189</v>
+        <v>201</v>
       </c>
       <c r="N35" t="s">
-        <v>194</v>
+        <v>201</v>
       </c>
       <c r="O35" t="s">
-        <v>203</v>
+        <v>210</v>
       </c>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.45">
@@ -7243,7 +7242,7 @@
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
-        <v>114</v>
+        <v>93</v>
       </c>
       <c r="B37" t="s">
         <v>94</v>
@@ -7258,19 +7257,19 @@
         <v>88</v>
       </c>
       <c r="F37" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="G37" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
       <c r="H37" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="I37" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
       <c r="J37">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="K37" t="s">
         <v>206</v>
@@ -7285,24 +7284,24 @@
         <v>201</v>
       </c>
       <c r="O37" t="s">
-        <v>28</v>
+        <v>204</v>
       </c>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
-        <v>142</v>
+        <v>114</v>
       </c>
       <c r="B38" t="s">
-        <v>148</v>
+        <v>94</v>
       </c>
       <c r="C38" t="s">
-        <v>8</v>
+        <v>87</v>
       </c>
       <c r="D38">
         <v>2017</v>
       </c>
       <c r="E38" t="s">
-        <v>3</v>
+        <v>88</v>
       </c>
       <c r="F38" t="s">
         <v>28</v>
@@ -7323,7 +7322,7 @@
         <v>206</v>
       </c>
       <c r="L38" t="s">
-        <v>3</v>
+        <v>209</v>
       </c>
       <c r="M38" t="s">
         <v>201</v>
@@ -7337,143 +7336,143 @@
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="B39" t="s">
-        <v>108</v>
+        <v>90</v>
       </c>
       <c r="C39" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D39">
         <v>2017</v>
       </c>
       <c r="E39" t="s">
-        <v>3</v>
+        <v>88</v>
       </c>
       <c r="F39" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="G39" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="H39" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
       <c r="I39" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
       <c r="J39">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K39" t="s">
         <v>206</v>
       </c>
       <c r="L39" t="s">
-        <v>3</v>
+        <v>209</v>
       </c>
       <c r="M39" t="s">
-        <v>201</v>
+        <v>191</v>
       </c>
       <c r="N39" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="O39" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
-        <v>35</v>
+        <v>89</v>
       </c>
       <c r="B40" t="s">
-        <v>50</v>
+        <v>90</v>
       </c>
       <c r="C40" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D40">
-        <v>2015</v>
+        <v>2017</v>
       </c>
       <c r="E40" t="s">
-        <v>3</v>
+        <v>88</v>
       </c>
       <c r="F40" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
       <c r="G40" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
       <c r="H40" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
       <c r="I40" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
       <c r="J40">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="K40" t="s">
         <v>206</v>
       </c>
       <c r="L40" t="s">
-        <v>3</v>
+        <v>209</v>
       </c>
       <c r="M40" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="N40" t="s">
-        <v>194</v>
+        <v>199</v>
       </c>
       <c r="O40" t="s">
-        <v>28</v>
+        <v>210</v>
       </c>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
-        <v>34</v>
+        <v>91</v>
       </c>
       <c r="B41" t="s">
-        <v>49</v>
+        <v>90</v>
       </c>
       <c r="C41" t="s">
         <v>13</v>
       </c>
       <c r="D41">
-        <v>2014</v>
+        <v>2017</v>
       </c>
       <c r="E41" t="s">
-        <v>102</v>
+        <v>88</v>
       </c>
       <c r="F41" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
       <c r="G41" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
       <c r="H41" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
       <c r="I41" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
       <c r="J41">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="K41" t="s">
         <v>206</v>
       </c>
       <c r="L41" t="s">
-        <v>4</v>
+        <v>209</v>
       </c>
       <c r="M41" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="N41" t="s">
         <v>194</v>
       </c>
       <c r="O41" t="s">
-        <v>28</v>
+        <v>210</v>
       </c>
     </row>
   </sheetData>
@@ -9096,21 +9095,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010038EC5152544FA941B2FCF6FC911C1211" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c0a7b694108ffeb4d5e14fa8f2f5e4a2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="f38ef60c-44b8-4b3e-b84e-3f774f47ec01" xmlns:ns4="77420ce7-ad61-40a5-b28d-42d2f2a680a0" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7cc2d357fdf517c32b7ae6696f0078b7" ns3:_="" ns4:_="">
     <xsd:import namespace="f38ef60c-44b8-4b3e-b84e-3f774f47ec01"/>
@@ -9333,32 +9317,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7AB5AB63-4FEC-4580-8B0C-E2F5F38CD9AC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="77420ce7-ad61-40a5-b28d-42d2f2a680a0"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="f38ef60c-44b8-4b3e-b84e-3f774f47ec01"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AB53F716-BD83-4083-9021-A1BA86EE45D6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5E51EC21-F22B-490E-8776-BB08FE496BF5}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9375,4 +9349,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AB53F716-BD83-4083-9021-A1BA86EE45D6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7AB5AB63-4FEC-4580-8B0C-E2F5F38CD9AC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="f38ef60c-44b8-4b3e-b84e-3f774f47ec01"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="77420ce7-ad61-40a5-b28d-42d2f2a680a0"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updated consistent olour mapping of all figures
</commit_message>
<xml_diff>
--- a/sample_info/A_rabiei_isolate_list_for_wgs.xlsx
+++ b/sample_info/A_rabiei_isolate_list_for_wgs.xlsx
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="306">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="313">
   <si>
     <t>Isolate</t>
   </si>
@@ -973,6 +973,27 @@
   </si>
   <si>
     <t xml:space="preserve">Elmore</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Patho.Group</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Group4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Group5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Group3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Group2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Group1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Group0</t>
   </si>
 </sst>
 </file>
@@ -995,12 +1016,12 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color theme="1"/>
       <name val="Calibri"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
     </font>
     <font>
@@ -1036,24 +1057,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF66"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor theme="4"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -1084,8 +1087,26 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFEE5F4C"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF66"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor theme="4"/>
       </patternFill>
     </fill>
     <fill>
@@ -1141,6 +1162,17 @@
       </bottom>
     </border>
     <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+    </border>
+    <border>
       <right style="thin">
         <color auto="1"/>
       </right>
@@ -1169,17 +1201,6 @@
       <bottom style="thin">
         <color auto="1"/>
       </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
     </border>
     <border>
       <left style="thin">
@@ -1251,55 +1272,36 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1308,61 +1310,80 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1374,33 +1395,33 @@
     <xf numFmtId="0" fontId="1" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2631,10 +2652,10 @@
 </table>
 </file>
 
-<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table8" displayName="Table8" ref="A1:K41" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A1:K41"/>
-  <tableColumns count="11">
+<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table9" displayName="Table9" ref="A1:L41" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A1:L41"/>
+  <tableColumns count="12">
     <tableColumn id="1" name="Isolate"/>
     <tableColumn id="2" name="Site"/>
     <tableColumn id="3" name="State"/>
@@ -2646,6 +2667,7 @@
     <tableColumn id="9" name="MAT_Type"/>
     <tableColumn id="10" name="Haplotype"/>
     <tableColumn id="11" name="Pathotype"/>
+    <tableColumn id="12" name="Patho.Group"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2995,1099 +3017,1099 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="21" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="21" t="s">
         <v>116</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="21" t="s">
         <v>83</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1" s="5" t="s">
+      <c r="G1" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="J1" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="K1" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="L1" s="21" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="12" t="n">
+      <c r="D2" s="4" t="n">
         <v>2013</v>
       </c>
-      <c r="E2" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" s="18" t="s">
+      <c r="E2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="H2" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="I2" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="J2" s="21" t="n">
+      <c r="G2" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="J2" s="14" t="n">
         <v>4</v>
       </c>
-      <c r="K2" s="12" t="s">
+      <c r="K2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="L2" s="12" t="s">
+      <c r="L2" s="4" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="12" t="n">
+      <c r="D3" s="4" t="n">
         <v>2014</v>
       </c>
-      <c r="E3" s="12" t="s">
+      <c r="E3" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="F3" s="18" t="s">
+      <c r="F3" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="H3" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="I3" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="J3" s="21" t="n">
+      <c r="G3" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="I3" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="J3" s="14" t="n">
         <v>4</v>
       </c>
-      <c r="K3" s="12" t="s">
+      <c r="K3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="L3" s="12" t="s">
+      <c r="L3" s="4" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="12" t="n">
+      <c r="D4" s="4" t="n">
         <v>2015</v>
       </c>
-      <c r="E4" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="F4" s="18" t="s">
+      <c r="E4" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="H4" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="I4" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="J4" s="21" t="n">
+      <c r="G4" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="I4" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="J4" s="14" t="n">
         <v>4</v>
       </c>
-      <c r="K4" s="12" t="s">
+      <c r="K4" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="L4" s="12" t="s">
+      <c r="L4" s="4" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="12" t="n">
+      <c r="D5" s="4" t="n">
         <v>2015</v>
       </c>
-      <c r="E5" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="F5" s="18" t="s">
+      <c r="E5" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F5" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="G5" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="H5" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="I5" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="J5" s="21" t="n">
+      <c r="G5" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="I5" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="J5" s="14" t="n">
         <v>4</v>
       </c>
-      <c r="K5" s="12" t="s">
+      <c r="K5" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="L5" s="12" t="s">
+      <c r="L5" s="4" t="s">
         <v>205</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="25" t="s">
         <v>92</v>
       </c>
-      <c r="B6" s="17" t="s">
+      <c r="B6" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="C6" s="17" t="s">
+      <c r="C6" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="17" t="n">
+      <c r="D6" s="9" t="n">
         <v>2016</v>
       </c>
-      <c r="E6" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="F6" s="25" t="s">
+      <c r="E6" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="F6" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="G6" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="H6" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="I6" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="J6" s="21" t="n">
+      <c r="G6" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="H6" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="I6" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="J6" s="14" t="n">
         <v>4</v>
       </c>
-      <c r="K6" s="17"/>
-      <c r="L6" s="12" t="s">
+      <c r="K6" s="9"/>
+      <c r="L6" s="4" t="s">
         <v>206</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="24" t="s">
         <v>89</v>
       </c>
-      <c r="B7" s="12" t="s">
+      <c r="B7" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="12" t="n">
+      <c r="D7" s="4" t="n">
         <v>2017</v>
       </c>
-      <c r="E7" s="12" t="s">
+      <c r="E7" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="F7" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="G7" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="H7" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="I7" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="J7" s="21" t="n">
+      <c r="F7" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="H7" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="I7" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="J7" s="14" t="n">
         <v>4</v>
       </c>
-      <c r="K7" s="12"/>
-      <c r="L7" s="12" t="s">
+      <c r="K7" s="4"/>
+      <c r="L7" s="4" t="s">
         <v>206</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="25" t="s">
         <v>91</v>
       </c>
-      <c r="B8" s="17" t="s">
+      <c r="B8" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="C8" s="17" t="s">
+      <c r="C8" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="17" t="n">
+      <c r="D8" s="9" t="n">
         <v>2017</v>
       </c>
-      <c r="E8" s="17" t="s">
+      <c r="E8" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="F8" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="G8" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="H8" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="I8" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="J8" s="21" t="n">
+      <c r="F8" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="H8" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="I8" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="J8" s="14" t="n">
         <v>4</v>
       </c>
-      <c r="K8" s="17"/>
-      <c r="L8" s="12" t="s">
+      <c r="K8" s="9"/>
+      <c r="L8" s="4" t="s">
         <v>206</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="25" t="s">
         <v>85</v>
       </c>
-      <c r="B9" s="17" t="s">
+      <c r="B9" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="C9" s="17" t="s">
+      <c r="C9" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="D9" s="17" t="n">
+      <c r="D9" s="9" t="n">
         <v>2017</v>
       </c>
-      <c r="E9" s="17" t="s">
+      <c r="E9" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="F9" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="G9" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="H9" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="I9" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="J9" s="21" t="n">
+      <c r="F9" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="H9" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="I9" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="J9" s="14" t="n">
         <v>4</v>
       </c>
-      <c r="K9" s="17"/>
-      <c r="L9" s="12" t="s">
+      <c r="K9" s="9"/>
+      <c r="L9" s="4" t="s">
         <v>206</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="25" t="s">
         <v>84</v>
       </c>
-      <c r="B10" s="17" t="s">
+      <c r="B10" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="C10" s="17" t="s">
+      <c r="C10" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="17" t="n">
+      <c r="D10" s="9" t="n">
         <v>2017</v>
       </c>
-      <c r="E10" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="F10" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="G10" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="H10" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="I10" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="J10" s="21" t="n">
+      <c r="E10" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="F10" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="G10" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="H10" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="I10" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="J10" s="14" t="n">
         <v>4</v>
       </c>
-      <c r="K10" s="17"/>
-      <c r="L10" s="12" t="s">
+      <c r="K10" s="9"/>
+      <c r="L10" s="4" t="s">
         <v>206</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="9" t="s">
+      <c r="A11" s="25" t="s">
         <v>72</v>
       </c>
-      <c r="B11" s="17" t="s">
+      <c r="B11" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="17" t="s">
+      <c r="C11" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="D11" s="17" t="n">
+      <c r="D11" s="9" t="n">
         <v>2013</v>
       </c>
-      <c r="E11" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="F11" s="18" t="s">
+      <c r="E11" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="F11" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="G11" s="18" t="s">
+      <c r="G11" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="H11" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="I11" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="J11" s="21" t="n">
-        <v>3</v>
-      </c>
-      <c r="K11" s="17" t="s">
+      <c r="H11" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="I11" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="J11" s="14" t="n">
+        <v>3</v>
+      </c>
+      <c r="K11" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="L11" s="12" t="s">
+      <c r="L11" s="4" t="s">
         <v>206</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="9" t="s">
+      <c r="A12" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="B12" s="17" t="s">
+      <c r="B12" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="C12" s="17" t="s">
+      <c r="C12" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="D12" s="17" t="n">
+      <c r="D12" s="9" t="n">
         <v>2015</v>
       </c>
-      <c r="E12" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="F12" s="18" t="s">
+      <c r="E12" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="F12" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="G12" s="18" t="s">
+      <c r="G12" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="H12" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="I12" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="J12" s="21" t="n">
-        <v>3</v>
-      </c>
-      <c r="K12" s="17" t="s">
+      <c r="H12" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="I12" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="J12" s="14" t="n">
+        <v>3</v>
+      </c>
+      <c r="K12" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="L12" s="12" t="s">
+      <c r="L12" s="4" t="s">
         <v>206</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="8" t="s">
+      <c r="A13" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="12" t="s">
+      <c r="B13" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C13" s="12" t="s">
+      <c r="C13" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D13" s="12" t="n">
+      <c r="D13" s="4" t="n">
         <v>2015</v>
       </c>
-      <c r="E13" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="F13" s="18" t="s">
+      <c r="E13" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F13" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="G13" s="18" t="s">
+      <c r="G13" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="H13" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="I13" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="J13" s="21" t="n">
-        <v>3</v>
-      </c>
-      <c r="K13" s="12" t="s">
+      <c r="H13" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="I13" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="J13" s="14" t="n">
+        <v>3</v>
+      </c>
+      <c r="K13" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="L13" s="12" t="s">
+      <c r="L13" s="4" t="s">
         <v>206</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="9" t="s">
+      <c r="A14" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="B14" s="17" t="s">
+      <c r="B14" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="C14" s="17" t="s">
+      <c r="C14" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="D14" s="17" t="n">
+      <c r="D14" s="9" t="n">
         <v>2015</v>
       </c>
-      <c r="E14" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="F14" s="18" t="s">
+      <c r="E14" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="F14" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="G14" s="18" t="s">
+      <c r="G14" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="H14" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="I14" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="J14" s="21" t="n">
-        <v>3</v>
-      </c>
-      <c r="K14" s="17" t="s">
+      <c r="H14" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="I14" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="J14" s="14" t="n">
+        <v>3</v>
+      </c>
+      <c r="K14" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="L14" s="12" t="s">
+      <c r="L14" s="4" t="s">
         <v>206</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="8" t="s">
+      <c r="A15" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="B15" s="12" t="s">
+      <c r="B15" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="C15" s="12" t="s">
+      <c r="C15" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D15" s="12" t="n">
+      <c r="D15" s="4" t="n">
         <v>2015</v>
       </c>
-      <c r="E15" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="F15" s="20" t="s">
+      <c r="E15" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F15" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="G15" s="20" t="s">
+      <c r="G15" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="H15" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="I15" s="24" t="s">
+      <c r="H15" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="I15" s="17" t="s">
         <v>79</v>
       </c>
-      <c r="J15" s="2" t="n">
-        <v>3</v>
-      </c>
-      <c r="K15" s="12" t="s">
+      <c r="J15" s="12" t="n">
+        <v>3</v>
+      </c>
+      <c r="K15" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="L15" s="12" t="s">
+      <c r="L15" s="4" t="s">
         <v>206</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="9" t="s">
+      <c r="A16" s="25" t="s">
         <v>78</v>
       </c>
-      <c r="B16" s="17" t="s">
+      <c r="B16" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="C16" s="17" t="s">
+      <c r="C16" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="D16" s="17" t="n">
+      <c r="D16" s="9" t="n">
         <v>2015</v>
       </c>
-      <c r="E16" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="F16" s="20" t="s">
+      <c r="E16" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="F16" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="G16" s="20" t="s">
+      <c r="G16" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="H16" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="I16" s="24" t="s">
+      <c r="H16" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="I16" s="17" t="s">
         <v>79</v>
       </c>
-      <c r="J16" s="2" t="n">
-        <v>3</v>
-      </c>
-      <c r="K16" s="17" t="s">
+      <c r="J16" s="12" t="n">
+        <v>3</v>
+      </c>
+      <c r="K16" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="L16" s="12" t="s">
+      <c r="L16" s="4" t="s">
         <v>206</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="8" t="s">
+      <c r="A17" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="B17" s="12" t="s">
+      <c r="B17" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="C17" s="12" t="s">
+      <c r="C17" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D17" s="12" t="n">
+      <c r="D17" s="4" t="n">
         <v>2015</v>
       </c>
-      <c r="E17" s="12" t="s">
+      <c r="E17" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="F17" s="18" t="s">
+      <c r="F17" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="G17" s="18" t="s">
+      <c r="G17" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="H17" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="I17" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="J17" s="2" t="n">
-        <v>3</v>
-      </c>
-      <c r="K17" s="12" t="s">
+      <c r="H17" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="I17" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="J17" s="12" t="n">
+        <v>3</v>
+      </c>
+      <c r="K17" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="L17" s="12" t="s">
+      <c r="L17" s="4" t="s">
         <v>206</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="9" t="s">
+      <c r="A18" s="25" t="s">
         <v>97</v>
       </c>
-      <c r="B18" s="17" t="s">
+      <c r="B18" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="C18" s="17" t="s">
+      <c r="C18" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="D18" s="17" t="n">
+      <c r="D18" s="9" t="n">
         <v>2016</v>
       </c>
-      <c r="E18" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="F18" s="25" t="s">
+      <c r="E18" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="F18" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="G18" s="25" t="s">
+      <c r="G18" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="H18" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="I18" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="J18" s="3" t="n">
-        <v>3</v>
-      </c>
-      <c r="K18" s="17"/>
-      <c r="L18" s="12" t="s">
+      <c r="H18" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="I18" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="J18" s="19" t="n">
+        <v>3</v>
+      </c>
+      <c r="K18" s="9"/>
+      <c r="L18" s="4" t="s">
         <v>206</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="8" t="s">
+      <c r="A19" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="B19" s="12" t="s">
+      <c r="B19" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="C19" s="12" t="s">
+      <c r="C19" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D19" s="12" t="n">
+      <c r="D19" s="4" t="n">
         <v>2016</v>
       </c>
-      <c r="E19" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="F19" s="25" t="s">
+      <c r="E19" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F19" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="G19" s="25" t="s">
+      <c r="G19" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="H19" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="I19" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="J19" s="3" t="n">
-        <v>3</v>
-      </c>
-      <c r="K19" s="12"/>
-      <c r="L19" s="12" t="s">
+      <c r="H19" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="I19" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="J19" s="19" t="n">
+        <v>3</v>
+      </c>
+      <c r="K19" s="4"/>
+      <c r="L19" s="4" t="s">
         <v>206</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="9" t="s">
+      <c r="A20" s="25" t="s">
         <v>75</v>
       </c>
-      <c r="B20" s="17" t="s">
+      <c r="B20" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="C20" s="17" t="s">
+      <c r="C20" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="D20" s="17" t="n">
+      <c r="D20" s="9" t="n">
         <v>2016</v>
       </c>
-      <c r="E20" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="F20" s="18" t="s">
+      <c r="E20" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="F20" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="G20" s="18" t="s">
+      <c r="G20" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="H20" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="I20" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="J20" s="2" t="n">
-        <v>3</v>
-      </c>
-      <c r="K20" s="17" t="s">
+      <c r="H20" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="I20" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="J20" s="12" t="n">
+        <v>3</v>
+      </c>
+      <c r="K20" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="L20" s="12" t="s">
+      <c r="L20" s="4" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="8" t="s">
+      <c r="A21" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="B21" s="12" t="s">
+      <c r="B21" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="C21" s="12" t="s">
+      <c r="C21" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D21" s="12" t="n">
+      <c r="D21" s="4" t="n">
         <v>2016</v>
       </c>
-      <c r="E21" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="F21" s="18" t="s">
+      <c r="E21" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F21" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="G21" s="18" t="s">
+      <c r="G21" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="H21" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="I21" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="J21" s="2" t="n">
-        <v>3</v>
-      </c>
-      <c r="K21" s="12" t="s">
+      <c r="H21" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="I21" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="J21" s="12" t="n">
+        <v>3</v>
+      </c>
+      <c r="K21" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="L21" s="12" t="s">
+      <c r="L21" s="4" t="s">
         <v>206</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="9" t="s">
+      <c r="A22" s="25" t="s">
         <v>95</v>
       </c>
-      <c r="B22" s="17" t="s">
+      <c r="B22" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="C22" s="17" t="s">
+      <c r="C22" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="D22" s="17" t="n">
+      <c r="D22" s="9" t="n">
         <v>2017</v>
       </c>
-      <c r="E22" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="F22" s="25" t="s">
+      <c r="E22" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="F22" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="G22" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="H22" s="25" t="s">
+      <c r="G22" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="H22" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="I22" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="J22" s="3" t="n">
-        <v>3</v>
-      </c>
-      <c r="K22" s="17"/>
-      <c r="L22" s="12" t="s">
+      <c r="I22" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="J22" s="19" t="n">
+        <v>3</v>
+      </c>
+      <c r="K22" s="9"/>
+      <c r="L22" s="4" t="s">
         <v>206</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="9" t="s">
+      <c r="A23" s="25" t="s">
         <v>98</v>
       </c>
-      <c r="B23" s="17" t="s">
+      <c r="B23" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="C23" s="17" t="s">
+      <c r="C23" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="D23" s="17" t="n">
+      <c r="D23" s="9" t="n">
         <v>2017</v>
       </c>
-      <c r="E23" s="17" t="s">
+      <c r="E23" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="F23" s="25" t="s">
+      <c r="F23" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="G23" s="25" t="s">
+      <c r="G23" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="H23" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="I23" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="J23" s="3" t="n">
-        <v>3</v>
-      </c>
-      <c r="K23" s="17"/>
-      <c r="L23" s="12" t="s">
+      <c r="H23" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="I23" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="J23" s="19" t="n">
+        <v>3</v>
+      </c>
+      <c r="K23" s="9"/>
+      <c r="L23" s="4" t="s">
         <v>206</v>
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="9" t="s">
+      <c r="A24" s="25" t="s">
         <v>93</v>
       </c>
-      <c r="B24" s="17" t="s">
+      <c r="B24" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="C24" s="17" t="s">
+      <c r="C24" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="D24" s="17" t="n">
+      <c r="D24" s="9" t="n">
         <v>2017</v>
       </c>
-      <c r="E24" s="17" t="s">
+      <c r="E24" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="F24" s="25" t="s">
+      <c r="F24" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="G24" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="H24" s="25" t="s">
+      <c r="G24" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="H24" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="I24" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="J24" s="3" t="n">
-        <v>3</v>
-      </c>
-      <c r="K24" s="17"/>
-      <c r="L24" s="12" t="s">
+      <c r="I24" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="J24" s="19" t="n">
+        <v>3</v>
+      </c>
+      <c r="K24" s="9"/>
+      <c r="L24" s="4" t="s">
         <v>206</v>
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="8" t="s">
+      <c r="A25" s="24" t="s">
         <v>113</v>
       </c>
-      <c r="B25" s="12" t="s">
+      <c r="B25" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="C25" s="12" t="s">
+      <c r="C25" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D25" s="12" t="n">
+      <c r="D25" s="4" t="n">
         <v>2017</v>
       </c>
-      <c r="E25" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="F25" s="18" t="s">
+      <c r="E25" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F25" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="G25" s="18" t="s">
+      <c r="G25" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="H25" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="I25" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="J25" s="7" t="n">
-        <v>3</v>
-      </c>
-      <c r="K25" s="12"/>
-      <c r="L25" s="12" t="s">
+      <c r="H25" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="I25" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="J25" s="23" t="n">
+        <v>3</v>
+      </c>
+      <c r="K25" s="4"/>
+      <c r="L25" s="4" t="s">
         <v>206</v>
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="8" t="s">
+      <c r="A26" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="B26" s="12" t="s">
+      <c r="B26" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C26" s="12" t="s">
+      <c r="C26" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D26" s="12" t="n">
+      <c r="D26" s="4" t="n">
         <v>2013</v>
       </c>
-      <c r="E26" s="12" t="s">
+      <c r="E26" s="4" t="s">
         <v>3</v>
       </c>
       <c r="F26" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="G26" s="18" t="s">
+      <c r="G26" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="H26" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="I26" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="J26" s="2" t="n">
+      <c r="H26" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="I26" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="J26" s="12" t="n">
         <v>2</v>
       </c>
-      <c r="K26" s="12" t="s">
+      <c r="K26" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="L26" s="12" t="s">
+      <c r="L26" s="4" t="s">
         <v>206</v>
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="9" t="s">
+      <c r="A27" s="25" t="s">
         <v>74</v>
       </c>
-      <c r="B27" s="17" t="s">
+      <c r="B27" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="C27" s="17" t="s">
+      <c r="C27" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="D27" s="17" t="n">
+      <c r="D27" s="9" t="n">
         <v>2015</v>
       </c>
-      <c r="E27" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="F27" s="19" t="s">
+      <c r="E27" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="F27" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="G27" s="20" t="s">
+      <c r="G27" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="H27" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="I27" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="J27" s="16" t="n">
+      <c r="H27" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="I27" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="J27" s="8" t="n">
         <v>2</v>
       </c>
-      <c r="K27" s="17" t="s">
+      <c r="K27" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="L27" s="12" t="s">
+      <c r="L27" s="4" t="s">
         <v>206</v>
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="8" t="s">
+      <c r="A28" s="24" t="s">
         <v>101</v>
       </c>
-      <c r="B28" s="12" t="s">
+      <c r="B28" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="C28" s="12" t="s">
+      <c r="C28" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D28" s="12" t="n">
+      <c r="D28" s="4" t="n">
         <v>2016</v>
       </c>
-      <c r="E28" s="12" t="s">
+      <c r="E28" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="F28" s="23" t="s">
+      <c r="F28" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="G28" s="25" t="s">
+      <c r="G28" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="H28" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="I28" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="J28" s="11" t="n">
+      <c r="H28" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="I28" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="J28" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="K28" s="12" t="s">
+      <c r="K28" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="L28" s="12" t="s">
+      <c r="L28" s="4" t="s">
         <v>206</v>
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="8" t="s">
+      <c r="A29" s="24" t="s">
         <v>99</v>
       </c>
-      <c r="B29" s="12" t="s">
+      <c r="B29" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="C29" s="12" t="s">
+      <c r="C29" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D29" s="12" t="n">
+      <c r="D29" s="4" t="n">
         <v>2016</v>
       </c>
-      <c r="E29" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="F29" s="23" t="s">
+      <c r="E29" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F29" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="G29" s="25" t="s">
+      <c r="G29" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="H29" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="I29" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="J29" s="15" t="n">
+      <c r="H29" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="I29" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="J29" s="7" t="n">
         <v>2</v>
       </c>
-      <c r="K29" s="12" t="s">
+      <c r="K29" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="L29" s="12" t="s">
+      <c r="L29" s="4" t="s">
         <v>206</v>
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="8" t="s">
+      <c r="A30" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="B30" s="12" t="s">
+      <c r="B30" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C30" s="12" t="s">
+      <c r="C30" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D30" s="12" t="n">
+      <c r="D30" s="4" t="n">
         <v>2014</v>
       </c>
-      <c r="E30" s="12" t="s">
+      <c r="E30" s="4" t="s">
         <v>102</v>
       </c>
       <c r="F30" s="1" t="s">
@@ -4096,36 +4118,36 @@
       <c r="G30" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="H30" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="I30" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="J30" s="2" t="n">
+      <c r="H30" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="I30" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="J30" s="12" t="n">
         <v>1</v>
       </c>
-      <c r="K30" s="12" t="s">
+      <c r="K30" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="L30" s="12" t="s">
+      <c r="L30" s="4" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="8" t="s">
+      <c r="A31" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="B31" s="12" t="s">
+      <c r="B31" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="C31" s="12" t="s">
+      <c r="C31" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D31" s="12" t="n">
+      <c r="D31" s="4" t="n">
         <v>2014</v>
       </c>
-      <c r="E31" s="12" t="s">
+      <c r="E31" s="4" t="s">
         <v>21</v>
       </c>
       <c r="F31" s="1" t="s">
@@ -4134,186 +4156,186 @@
       <c r="G31" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="H31" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="I31" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="J31" s="2" t="n">
+      <c r="H31" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="I31" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="J31" s="12" t="n">
         <v>1</v>
       </c>
-      <c r="K31" s="12" t="s">
+      <c r="K31" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="L31" s="12" t="s">
+      <c r="L31" s="4" t="s">
         <v>206</v>
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="9" t="s">
+      <c r="A32" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="B32" s="17" t="s">
+      <c r="B32" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="C32" s="17" t="s">
+      <c r="C32" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="D32" s="17" t="n">
+      <c r="D32" s="9" t="n">
         <v>2015</v>
       </c>
-      <c r="E32" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="F32" s="19" t="s">
+      <c r="E32" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="F32" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="G32" s="19" t="s">
+      <c r="G32" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="H32" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="I32" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="J32" s="2" t="n">
+      <c r="H32" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="I32" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="J32" s="12" t="n">
         <v>1</v>
       </c>
-      <c r="K32" s="17" t="s">
+      <c r="K32" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="L32" s="12" t="s">
+      <c r="L32" s="4" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="33">
-      <c r="A33" s="9" t="s">
+      <c r="A33" s="25" t="s">
         <v>143</v>
       </c>
-      <c r="B33" s="17" t="s">
+      <c r="B33" s="9" t="s">
         <v>145</v>
       </c>
-      <c r="C33" s="17" t="s">
+      <c r="C33" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="D33" s="17" t="n">
+      <c r="D33" s="9" t="n">
         <v>2016</v>
       </c>
-      <c r="E33" s="12" t="s">
+      <c r="E33" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="F33" s="23" t="s">
+      <c r="F33" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="G33" s="23" t="s">
+      <c r="G33" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="H33" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="I33" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="J33" s="10" t="n">
+      <c r="H33" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="I33" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="J33" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="K33" s="17"/>
-      <c r="L33" s="12" t="s">
+      <c r="K33" s="9"/>
+      <c r="L33" s="4" t="s">
         <v>206</v>
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="8" t="s">
+      <c r="A34" s="24" t="s">
         <v>104</v>
       </c>
-      <c r="B34" s="12" t="s">
+      <c r="B34" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="C34" s="12" t="s">
+      <c r="C34" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D34" s="12" t="n">
+      <c r="D34" s="4" t="n">
         <v>2016</v>
       </c>
-      <c r="E34" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="F34" s="23" t="s">
+      <c r="E34" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F34" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="G34" s="23" t="s">
+      <c r="G34" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="H34" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="I34" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="J34" s="13" t="n">
+      <c r="H34" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="I34" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="J34" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="K34" s="12" t="s">
+      <c r="K34" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="L34" s="12" t="s">
+      <c r="L34" s="4" t="s">
         <v>206</v>
       </c>
     </row>
     <row r="35">
-      <c r="A35" s="9" t="s">
+      <c r="A35" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="B35" s="17" t="s">
+      <c r="B35" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="C35" s="17" t="s">
+      <c r="C35" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="D35" s="17" t="n">
+      <c r="D35" s="9" t="n">
         <v>2016</v>
       </c>
-      <c r="E35" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="F35" s="23" t="s">
+      <c r="E35" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="F35" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="G35" s="23" t="s">
+      <c r="G35" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="H35" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="I35" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="J35" s="13" t="n">
+      <c r="H35" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="I35" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="J35" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="K35" s="12" t="s">
+      <c r="K35" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="L35" s="12" t="s">
+      <c r="L35" s="4" t="s">
         <v>206</v>
       </c>
     </row>
     <row r="36">
-      <c r="A36" s="9" t="s">
+      <c r="A36" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="B36" s="17" t="s">
+      <c r="B36" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="C36" s="17" t="s">
+      <c r="C36" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="D36" s="17" t="n">
+      <c r="D36" s="9" t="n">
         <v>2014</v>
       </c>
-      <c r="E36" s="17" t="s">
+      <c r="E36" s="9" t="s">
         <v>102</v>
       </c>
       <c r="F36" s="1" t="s">
@@ -4328,30 +4350,30 @@
       <c r="I36" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="J36" s="7" t="n">
+      <c r="J36" s="23" t="n">
         <v>0</v>
       </c>
-      <c r="K36" s="17" t="s">
+      <c r="K36" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="L36" s="12" t="s">
+      <c r="L36" s="4" t="s">
         <v>206</v>
       </c>
     </row>
     <row r="37">
-      <c r="A37" s="9" t="s">
+      <c r="A37" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="B37" s="17" t="s">
+      <c r="B37" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="C37" s="17" t="s">
+      <c r="C37" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="D37" s="17" t="n">
+      <c r="D37" s="9" t="n">
         <v>2015</v>
       </c>
-      <c r="E37" s="17" t="s">
+      <c r="E37" s="9" t="s">
         <v>3</v>
       </c>
       <c r="F37" s="1" t="s">
@@ -4366,66 +4388,66 @@
       <c r="I37" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="J37" s="7" t="n">
+      <c r="J37" s="23" t="n">
         <v>0</v>
       </c>
-      <c r="K37" s="17" t="s">
+      <c r="K37" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="L37" s="12" t="s">
+      <c r="L37" s="4" t="s">
         <v>206</v>
       </c>
     </row>
     <row r="38">
-      <c r="A38" s="8" t="s">
+      <c r="A38" s="24" t="s">
         <v>109</v>
       </c>
-      <c r="B38" s="12" t="s">
+      <c r="B38" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="C38" s="12" t="s">
+      <c r="C38" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="D38" s="12" t="n">
+      <c r="D38" s="4" t="n">
         <v>2017</v>
       </c>
-      <c r="E38" s="12" t="s">
+      <c r="E38" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="F38" s="23" t="s">
+      <c r="F38" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="G38" s="23" t="s">
+      <c r="G38" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="H38" s="23" t="s">
+      <c r="H38" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="I38" s="23" t="s">
+      <c r="I38" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="J38" s="10" t="n">
+      <c r="J38" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K38" s="12"/>
-      <c r="L38" s="12" t="s">
+      <c r="K38" s="4"/>
+      <c r="L38" s="4" t="s">
         <v>206</v>
       </c>
     </row>
     <row r="39">
-      <c r="A39" s="8" t="s">
+      <c r="A39" s="24" t="s">
         <v>114</v>
       </c>
-      <c r="B39" s="12" t="s">
+      <c r="B39" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="C39" s="12" t="s">
+      <c r="C39" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="D39" s="12" t="n">
+      <c r="D39" s="4" t="n">
         <v>2017</v>
       </c>
-      <c r="E39" s="12" t="s">
+      <c r="E39" s="4" t="s">
         <v>88</v>
       </c>
       <c r="F39" s="1" t="s">
@@ -4440,83 +4462,83 @@
       <c r="I39" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="J39" s="22" t="n">
+      <c r="J39" s="15" t="n">
         <v>0</v>
       </c>
-      <c r="K39" s="12"/>
-      <c r="L39" s="12" t="s">
+      <c r="K39" s="4"/>
+      <c r="L39" s="4" t="s">
         <v>206</v>
       </c>
     </row>
     <row r="40">
-      <c r="A40" s="9" t="s">
+      <c r="A40" s="25" t="s">
         <v>142</v>
       </c>
-      <c r="B40" s="17" t="s">
+      <c r="B40" s="9" t="s">
         <v>148</v>
       </c>
-      <c r="C40" s="17" t="s">
+      <c r="C40" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="D40" s="17" t="n">
+      <c r="D40" s="9" t="n">
         <v>2017</v>
       </c>
-      <c r="E40" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="F40" s="23" t="s">
+      <c r="E40" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F40" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="G40" s="23" t="s">
+      <c r="G40" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="H40" s="23" t="s">
+      <c r="H40" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="I40" s="23" t="s">
+      <c r="I40" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="J40" s="14" t="n">
+      <c r="J40" s="6" t="n">
         <v>0</v>
       </c>
-      <c r="K40" s="17"/>
-      <c r="L40" s="12" t="s">
+      <c r="K40" s="9"/>
+      <c r="L40" s="4" t="s">
         <v>206</v>
       </c>
     </row>
     <row r="41">
-      <c r="A41" s="12" t="s">
+      <c r="A41" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="B41" s="12" t="s">
+      <c r="B41" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="C41" s="12" t="s">
+      <c r="C41" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D41" s="12" t="n">
+      <c r="D41" s="4" t="n">
         <v>2017</v>
       </c>
-      <c r="E41" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="F41" s="23" t="s">
+      <c r="E41" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F41" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="G41" s="23" t="s">
+      <c r="G41" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="H41" s="23" t="s">
+      <c r="H41" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="I41" s="23" t="s">
+      <c r="I41" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="J41" s="10" t="n">
+      <c r="J41" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K41" s="12"/>
-      <c r="L41" s="12" t="s">
+      <c r="K41" s="4"/>
+      <c r="L41" s="4" t="s">
         <v>206</v>
       </c>
     </row>
@@ -4802,7 +4824,7 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="20" t="s">
         <v>117</v>
       </c>
       <c r="B1" s="31" t="s">
@@ -5688,10 +5710,10 @@
         <v>2017</v>
       </c>
       <c r="F2" s="36"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23"/>
-      <c r="I2" s="23"/>
-      <c r="J2" s="23"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="16"/>
+      <c r="I2" s="16"/>
+      <c r="J2" s="16"/>
       <c r="K2" s="39"/>
       <c r="L2" s="36"/>
       <c r="M2" s="36" t="s">
@@ -5717,10 +5739,10 @@
       <c r="F3" s="37" t="s">
         <v>102</v>
       </c>
-      <c r="G3" s="23"/>
-      <c r="H3" s="23"/>
-      <c r="I3" s="23"/>
-      <c r="J3" s="23"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="16"/>
+      <c r="I3" s="16"/>
+      <c r="J3" s="16"/>
       <c r="K3" s="39"/>
       <c r="L3" s="35"/>
       <c r="M3" s="35" t="s">
@@ -7903,16 +7925,16 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="4" t="s">
         <v>21</v>
       </c>
       <c r="E2" s="1" t="s">
@@ -7927,27 +7949,27 @@
       <c r="H2" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="I2" s="21" t="n">
+      <c r="I2" s="14" t="n">
         <v>1</v>
       </c>
-      <c r="J2" s="17" t="s">
+      <c r="J2" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="K2" s="17" t="s">
+      <c r="K2" s="9" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="C3" s="17" t="s">
+      <c r="C3" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="17" t="s">
+      <c r="D3" s="9" t="s">
         <v>31</v>
       </c>
       <c r="E3" s="1" t="s">
@@ -7965,26 +7987,26 @@
       <c r="I3" s="60" t="n">
         <v>1</v>
       </c>
-      <c r="J3" s="17"/>
-      <c r="K3" s="17"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="9"/>
     </row>
     <row r="4">
-      <c r="A4" s="17" t="s">
+      <c r="A4" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="B4" s="17" t="s">
+      <c r="B4" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="C4" s="17" t="s">
+      <c r="C4" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="E4" s="19" t="s">
+      <c r="D4" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="F4" s="20" t="s">
+      <c r="F4" s="13" t="s">
         <v>9</v>
       </c>
       <c r="G4" s="55" t="s">
@@ -7996,27 +8018,27 @@
       <c r="I4" s="59" t="n">
         <v>2</v>
       </c>
-      <c r="J4" s="17" t="s">
+      <c r="J4" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="K4" s="17" t="s">
+      <c r="K4" s="9" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="E5" s="18" t="s">
+      <c r="D5" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" s="10" t="s">
         <v>9</v>
       </c>
       <c r="F5" s="45" t="s">
@@ -8028,33 +8050,33 @@
       <c r="H5" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="I5" s="21" t="n">
+      <c r="I5" s="14" t="n">
         <v>4</v>
       </c>
       <c r="J5" s="46" t="s">
         <v>16</v>
       </c>
-      <c r="K5" s="17" t="s">
+      <c r="K5" s="9" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="12" t="s">
+      <c r="A6" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B6" s="17" t="s">
+      <c r="B6" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="12" t="s">
+      <c r="D6" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="E6" s="19" t="s">
+      <c r="E6" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="F6" s="19" t="s">
+      <c r="F6" s="11" t="s">
         <v>28</v>
       </c>
       <c r="G6" s="55" t="s">
@@ -8063,30 +8085,30 @@
       <c r="H6" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="I6" s="21" t="n">
+      <c r="I6" s="14" t="n">
         <v>1</v>
       </c>
-      <c r="J6" s="17" t="s">
+      <c r="J6" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="K6" s="17" t="s">
+      <c r="K6" s="9" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="17" t="s">
+      <c r="A7" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="17" t="s">
+      <c r="B7" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="C7" s="17" t="s">
+      <c r="C7" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="E7" s="18" t="s">
+      <c r="D7" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="E7" s="10" t="s">
         <v>9</v>
       </c>
       <c r="F7" s="45" t="s">
@@ -8098,27 +8120,27 @@
       <c r="H7" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="I7" s="21" t="n">
+      <c r="I7" s="14" t="n">
         <v>4</v>
       </c>
       <c r="J7" s="46" t="s">
         <v>18</v>
       </c>
-      <c r="K7" s="17" t="s">
+      <c r="K7" s="9" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="12" t="s">
+      <c r="A8" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B8" s="17" t="s">
+      <c r="B8" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C8" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="12" t="s">
+      <c r="D8" s="4" t="s">
         <v>3</v>
       </c>
       <c r="E8" s="1" t="s">
@@ -8133,33 +8155,33 @@
       <c r="H8" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="I8" s="22" t="n">
+      <c r="I8" s="15" t="n">
         <v>0</v>
       </c>
-      <c r="J8" s="17" t="s">
+      <c r="J8" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="K8" s="17" t="s">
+      <c r="K8" s="9" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="17" t="s">
+      <c r="A9" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="B9" s="17" t="s">
+      <c r="B9" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="C9" s="17" t="s">
+      <c r="C9" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="17" t="s">
+      <c r="D9" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="E9" s="18" t="s">
+      <c r="E9" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="F9" s="18" t="s">
+      <c r="F9" s="10" t="s">
         <v>9</v>
       </c>
       <c r="G9" s="45" t="s">
@@ -8168,30 +8190,30 @@
       <c r="H9" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="I9" s="21" t="n">
-        <v>3</v>
-      </c>
-      <c r="J9" s="17" t="s">
+      <c r="I9" s="14" t="n">
+        <v>3</v>
+      </c>
+      <c r="J9" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="K9" s="17" t="s">
+      <c r="K9" s="9" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="12" t="s">
+      <c r="A10" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="17" t="s">
+      <c r="B10" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="C10" s="12" t="s">
+      <c r="C10" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D10" s="12" t="s">
+      <c r="D10" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E10" s="18" t="s">
+      <c r="E10" s="10" t="s">
         <v>9</v>
       </c>
       <c r="F10" s="45" t="s">
@@ -8206,28 +8228,28 @@
       <c r="I10" s="60" t="n">
         <v>4</v>
       </c>
-      <c r="J10" s="17" t="s">
+      <c r="J10" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="K10" s="17"/>
+      <c r="K10" s="9"/>
     </row>
     <row r="11">
-      <c r="A11" s="12" t="s">
+      <c r="A11" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="B11" s="17" t="s">
+      <c r="B11" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="C11" s="12" t="s">
+      <c r="C11" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D11" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="E11" s="18" t="s">
+      <c r="D11" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E11" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="F11" s="18" t="s">
+      <c r="F11" s="10" t="s">
         <v>9</v>
       </c>
       <c r="G11" s="45" t="s">
@@ -8236,33 +8258,33 @@
       <c r="H11" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="I11" s="21" t="n">
-        <v>3</v>
-      </c>
-      <c r="J11" s="17" t="s">
+      <c r="I11" s="14" t="n">
+        <v>3</v>
+      </c>
+      <c r="J11" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="K11" s="17" t="s">
+      <c r="K11" s="9" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="17" t="s">
+      <c r="A12" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="B12" s="17" t="s">
+      <c r="B12" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="C12" s="17" t="s">
+      <c r="C12" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="D12" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="E12" s="18" t="s">
+      <c r="D12" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="E12" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="F12" s="18" t="s">
+      <c r="F12" s="10" t="s">
         <v>9</v>
       </c>
       <c r="G12" s="45" t="s">
@@ -8271,33 +8293,33 @@
       <c r="H12" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="I12" s="21" t="n">
-        <v>3</v>
-      </c>
-      <c r="J12" s="17" t="s">
+      <c r="I12" s="14" t="n">
+        <v>3</v>
+      </c>
+      <c r="J12" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="K12" s="17" t="s">
+      <c r="K12" s="9" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="12" t="s">
+      <c r="A13" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="B13" s="17" t="s">
+      <c r="B13" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="C13" s="12" t="s">
+      <c r="C13" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D13" s="12" t="s">
+      <c r="D13" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="E13" s="18" t="s">
+      <c r="E13" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="F13" s="18" t="s">
+      <c r="F13" s="10" t="s">
         <v>9</v>
       </c>
       <c r="G13" s="45" t="s">
@@ -8310,24 +8332,24 @@
         <v>3</v>
       </c>
       <c r="J13" s="56"/>
-      <c r="K13" s="17" t="s">
+      <c r="K13" s="9" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="17" t="s">
+      <c r="A14" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="B14" s="17" t="s">
+      <c r="B14" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C14" s="17" t="s">
+      <c r="C14" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="D14" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="E14" s="18" t="s">
+      <c r="D14" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="E14" s="10" t="s">
         <v>9</v>
       </c>
       <c r="F14" s="45" t="s">
@@ -8342,25 +8364,25 @@
       <c r="I14" s="60" t="n">
         <v>4</v>
       </c>
-      <c r="J14" s="17" t="s">
+      <c r="J14" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="K14" s="17"/>
+      <c r="K14" s="9"/>
     </row>
     <row r="15">
-      <c r="A15" s="17" t="s">
+      <c r="A15" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="B15" s="17" t="s">
+      <c r="B15" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="17" t="s">
+      <c r="C15" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="D15" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="E15" s="18" t="s">
+      <c r="D15" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="E15" s="10" t="s">
         <v>9</v>
       </c>
       <c r="F15" s="45" t="s">
@@ -8372,33 +8394,33 @@
       <c r="H15" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="I15" s="21" t="n">
+      <c r="I15" s="14" t="n">
         <v>4</v>
       </c>
-      <c r="J15" s="17" t="s">
+      <c r="J15" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="K15" s="17" t="s">
+      <c r="K15" s="9" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="12" t="s">
+      <c r="A16" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="B16" s="17" t="s">
+      <c r="B16" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C16" s="12" t="s">
+      <c r="C16" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D16" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="E16" s="18" t="s">
+      <c r="D16" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E16" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="F16" s="18" t="s">
+      <c r="F16" s="10" t="s">
         <v>9</v>
       </c>
       <c r="G16" s="45" t="s">
@@ -8407,33 +8429,33 @@
       <c r="H16" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="I16" s="21" t="n">
-        <v>3</v>
-      </c>
-      <c r="J16" s="17" t="s">
+      <c r="I16" s="14" t="n">
+        <v>3</v>
+      </c>
+      <c r="J16" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="K16" s="17" t="s">
+      <c r="K16" s="9" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="17" t="s">
+      <c r="A17" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="B17" s="17" t="s">
+      <c r="B17" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C17" s="17" t="s">
+      <c r="C17" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="D17" s="17" t="s">
+      <c r="D17" s="9" t="s">
         <v>3</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F17" s="18" t="s">
+      <c r="F17" s="10" t="s">
         <v>9</v>
       </c>
       <c r="G17" s="45" t="s">
@@ -8442,27 +8464,27 @@
       <c r="H17" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="I17" s="21" t="n">
+      <c r="I17" s="14" t="n">
         <v>2</v>
       </c>
-      <c r="J17" s="17" t="s">
+      <c r="J17" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="K17" s="17" t="s">
+      <c r="K17" s="9" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="12" t="s">
+      <c r="A18" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="B18" s="17" t="s">
+      <c r="B18" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="C18" s="12" t="s">
+      <c r="C18" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D18" s="12" t="s">
+      <c r="D18" s="4" t="s">
         <v>59</v>
       </c>
       <c r="E18" s="47" t="s">
@@ -8480,20 +8502,20 @@
       <c r="I18" s="60" t="n">
         <v>1</v>
       </c>
-      <c r="J18" s="17"/>
-      <c r="K18" s="17"/>
+      <c r="J18" s="9"/>
+      <c r="K18" s="9"/>
     </row>
     <row r="19">
-      <c r="A19" s="17" t="s">
+      <c r="A19" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="B19" s="17" t="s">
+      <c r="B19" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="C19" s="17" t="s">
+      <c r="C19" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="D19" s="17" t="s">
+      <c r="D19" s="9" t="s">
         <v>3</v>
       </c>
       <c r="E19" s="47" t="s">
@@ -8511,20 +8533,20 @@
       <c r="I19" s="60" t="n">
         <v>1</v>
       </c>
-      <c r="J19" s="17"/>
-      <c r="K19" s="17"/>
+      <c r="J19" s="9"/>
+      <c r="K19" s="9"/>
     </row>
     <row r="20">
-      <c r="A20" s="17" t="s">
+      <c r="A20" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="B20" s="17" t="s">
+      <c r="B20" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="C20" s="17" t="s">
+      <c r="C20" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="D20" s="17" t="s">
+      <c r="D20" s="9" t="s">
         <v>3</v>
       </c>
       <c r="E20" s="1" t="s">
@@ -8539,27 +8561,27 @@
       <c r="H20" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="I20" s="23" t="n">
+      <c r="I20" s="16" t="n">
         <v>0</v>
       </c>
-      <c r="J20" s="17" t="s">
+      <c r="J20" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="K20" s="17" t="s">
+      <c r="K20" s="9" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="12" t="s">
+      <c r="A21" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="B21" s="17" t="s">
+      <c r="B21" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="C21" s="12" t="s">
+      <c r="C21" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D21" s="12" t="s">
+      <c r="D21" s="4" t="s">
         <v>3</v>
       </c>
       <c r="E21" s="47" t="s">
@@ -8577,26 +8599,26 @@
       <c r="I21" s="60" t="n">
         <v>1</v>
       </c>
-      <c r="J21" s="17"/>
-      <c r="K21" s="17"/>
+      <c r="J21" s="9"/>
+      <c r="K21" s="9"/>
     </row>
     <row r="22">
-      <c r="A22" s="12" t="s">
+      <c r="A22" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B22" s="17" t="s">
+      <c r="B22" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="C22" s="12" t="s">
+      <c r="C22" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D22" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="E22" s="18" t="s">
+      <c r="D22" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E22" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="F22" s="18" t="s">
+      <c r="F22" s="10" t="s">
         <v>9</v>
       </c>
       <c r="G22" s="45" t="s">
@@ -8605,30 +8627,30 @@
       <c r="H22" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="I22" s="21" t="n">
-        <v>3</v>
-      </c>
-      <c r="J22" s="17" t="s">
+      <c r="I22" s="14" t="n">
+        <v>3</v>
+      </c>
+      <c r="J22" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="K22" s="17" t="s">
+      <c r="K22" s="9" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="17" t="s">
+      <c r="A23" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B23" s="17" t="s">
+      <c r="B23" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="C23" s="17" t="s">
+      <c r="C23" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="D23" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="E23" s="18" t="s">
+      <c r="D23" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="E23" s="10" t="s">
         <v>9</v>
       </c>
       <c r="F23" s="45" t="s">
@@ -8643,28 +8665,28 @@
       <c r="I23" s="60" t="n">
         <v>4</v>
       </c>
-      <c r="J23" s="17" t="s">
+      <c r="J23" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="K23" s="17"/>
+      <c r="K23" s="9"/>
     </row>
     <row r="24">
-      <c r="A24" s="17" t="s">
+      <c r="A24" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="B24" s="17" t="s">
+      <c r="B24" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="C24" s="17" t="s">
+      <c r="C24" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="D24" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="E24" s="18" t="s">
+      <c r="D24" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="E24" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="F24" s="18" t="s">
+      <c r="F24" s="10" t="s">
         <v>9</v>
       </c>
       <c r="G24" s="45" t="s">
@@ -8673,33 +8695,33 @@
       <c r="H24" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="I24" s="21" t="n">
-        <v>3</v>
-      </c>
-      <c r="J24" s="17" t="s">
+      <c r="I24" s="14" t="n">
+        <v>3</v>
+      </c>
+      <c r="J24" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="K24" s="17" t="s">
+      <c r="K24" s="9" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="12" t="s">
+      <c r="A25" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B25" s="17" t="s">
+      <c r="B25" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="C25" s="12" t="s">
+      <c r="C25" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D25" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="E25" s="18" t="s">
+      <c r="D25" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E25" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="F25" s="18" t="s">
+      <c r="F25" s="10" t="s">
         <v>9</v>
       </c>
       <c r="G25" s="45" t="s">
@@ -8708,33 +8730,33 @@
       <c r="H25" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="I25" s="21" t="n">
+      <c r="I25" s="14" t="n">
         <v>3</v>
       </c>
       <c r="J25" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="K25" s="17" t="s">
+      <c r="K25" s="9" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="17" t="s">
+      <c r="A26" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="B26" s="17" t="s">
+      <c r="B26" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="C26" s="17" t="s">
+      <c r="C26" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="D26" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="E26" s="20" t="s">
+      <c r="D26" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="E26" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="F26" s="20" t="s">
+      <c r="F26" s="13" t="s">
         <v>9</v>
       </c>
       <c r="G26" s="55" t="s">
@@ -8743,33 +8765,33 @@
       <c r="H26" s="45" t="s">
         <v>79</v>
       </c>
-      <c r="I26" s="21" t="n">
-        <v>3</v>
-      </c>
-      <c r="J26" s="17" t="s">
+      <c r="I26" s="14" t="n">
+        <v>3</v>
+      </c>
+      <c r="J26" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="K26" s="17" t="s">
+      <c r="K26" s="9" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="12" t="s">
+      <c r="A27" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="B27" s="17" t="s">
+      <c r="B27" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="C27" s="12" t="s">
+      <c r="C27" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D27" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="E27" s="20" t="s">
+      <c r="D27" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E27" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="F27" s="20" t="s">
+      <c r="F27" s="13" t="s">
         <v>9</v>
       </c>
       <c r="G27" s="55" t="s">
@@ -8778,27 +8800,27 @@
       <c r="H27" s="45" t="s">
         <v>79</v>
       </c>
-      <c r="I27" s="21" t="n">
-        <v>3</v>
-      </c>
-      <c r="J27" s="17" t="s">
+      <c r="I27" s="14" t="n">
+        <v>3</v>
+      </c>
+      <c r="J27" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="K27" s="17" t="s">
+      <c r="K27" s="9" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="17" t="s">
+      <c r="A28" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="B28" s="17" t="s">
+      <c r="B28" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="C28" s="17" t="s">
+      <c r="C28" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="D28" s="17" t="s">
+      <c r="D28" s="9" t="s">
         <v>4</v>
       </c>
       <c r="E28" s="1" t="s">
@@ -8813,27 +8835,27 @@
       <c r="H28" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="I28" s="21" t="n">
+      <c r="I28" s="14" t="n">
         <v>1</v>
       </c>
-      <c r="J28" s="17" t="s">
+      <c r="J28" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="K28" s="17" t="s">
+      <c r="K28" s="9" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="12" t="s">
+      <c r="A29" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B29" s="17" t="s">
+      <c r="B29" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="C29" s="12" t="s">
+      <c r="C29" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D29" s="12" t="s">
+      <c r="D29" s="4" t="s">
         <v>4</v>
       </c>
       <c r="E29" s="1" t="s">
@@ -8848,27 +8870,27 @@
       <c r="H29" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="I29" s="22" t="n">
+      <c r="I29" s="15" t="n">
         <v>0</v>
       </c>
-      <c r="J29" s="17" t="s">
+      <c r="J29" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="K29" s="17" t="s">
+      <c r="K29" s="9" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="12" t="s">
+      <c r="A30" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B30" s="17" t="s">
+      <c r="B30" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="C30" s="12" t="s">
+      <c r="C30" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D30" s="12" t="s">
+      <c r="D30" s="4" t="s">
         <v>4</v>
       </c>
       <c r="E30" s="48" t="s">
@@ -8892,19 +8914,19 @@
       <c r="K30" s="54"/>
     </row>
     <row r="31">
-      <c r="A31" s="17" t="s">
+      <c r="A31" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="B31" s="17" t="s">
+      <c r="B31" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="C31" s="17" t="s">
+      <c r="C31" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="D31" s="17" t="s">
+      <c r="D31" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="E31" s="18" t="s">
+      <c r="E31" s="10" t="s">
         <v>9</v>
       </c>
       <c r="F31" s="51" t="s">
@@ -8927,16 +8949,16 @@
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="17" t="s">
+      <c r="A32" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="B32" s="17" t="s">
+      <c r="B32" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="C32" s="17" t="s">
+      <c r="C32" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="D32" s="17" t="s">
+      <c r="D32" s="9" t="s">
         <v>4</v>
       </c>
       <c r="E32" s="49" t="s">
@@ -8960,16 +8982,16 @@
       <c r="K32" s="54"/>
     </row>
     <row r="33">
-      <c r="A33" s="12" t="s">
+      <c r="A33" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="B33" s="17" t="s">
+      <c r="B33" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="C33" s="12" t="s">
+      <c r="C33" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D33" s="12" t="s">
+      <c r="D33" s="4" t="s">
         <v>4</v>
       </c>
       <c r="E33" s="50" t="s">
@@ -10819,6 +10841,9 @@
       <c r="K1" t="s">
         <v>221</v>
       </c>
+      <c r="L1" t="s">
+        <v>306</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
@@ -10854,6 +10879,9 @@
       <c r="K2" t="s">
         <v>230</v>
       </c>
+      <c r="L2" t="s">
+        <v>307</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
@@ -10889,6 +10917,9 @@
       <c r="K3" t="s">
         <v>230</v>
       </c>
+      <c r="L3" t="s">
+        <v>307</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
@@ -10924,6 +10955,9 @@
       <c r="K4" t="s">
         <v>230</v>
       </c>
+      <c r="L4" t="s">
+        <v>307</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
@@ -10959,6 +10993,9 @@
       <c r="K5" t="s">
         <v>230</v>
       </c>
+      <c r="L5" t="s">
+        <v>307</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
@@ -10994,6 +11031,9 @@
       <c r="K6" t="s">
         <v>230</v>
       </c>
+      <c r="L6" t="s">
+        <v>307</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
@@ -11029,6 +11069,9 @@
       <c r="K7" t="s">
         <v>250</v>
       </c>
+      <c r="L7" t="s">
+        <v>308</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
@@ -11064,6 +11107,9 @@
       <c r="K8" t="s">
         <v>250</v>
       </c>
+      <c r="L8" t="s">
+        <v>308</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
@@ -11099,6 +11145,9 @@
       <c r="K9" t="s">
         <v>250</v>
       </c>
+      <c r="L9" t="s">
+        <v>308</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
@@ -11134,6 +11183,9 @@
       <c r="K10" t="s">
         <v>250</v>
       </c>
+      <c r="L10" t="s">
+        <v>308</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
@@ -11169,6 +11221,9 @@
       <c r="K11" t="s">
         <v>226</v>
       </c>
+      <c r="L11" t="s">
+        <v>309</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
@@ -11204,6 +11259,9 @@
       <c r="K12" t="s">
         <v>226</v>
       </c>
+      <c r="L12" t="s">
+        <v>309</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
@@ -11239,6 +11297,9 @@
       <c r="K13" t="s">
         <v>226</v>
       </c>
+      <c r="L13" t="s">
+        <v>309</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
@@ -11274,6 +11335,9 @@
       <c r="K14" t="s">
         <v>226</v>
       </c>
+      <c r="L14" t="s">
+        <v>309</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
@@ -11309,6 +11373,9 @@
       <c r="K15" t="s">
         <v>226</v>
       </c>
+      <c r="L15" t="s">
+        <v>309</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
@@ -11344,6 +11411,9 @@
       <c r="K16" t="s">
         <v>226</v>
       </c>
+      <c r="L16" t="s">
+        <v>309</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
@@ -11379,6 +11449,9 @@
       <c r="K17" t="s">
         <v>226</v>
       </c>
+      <c r="L17" t="s">
+        <v>309</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
@@ -11414,6 +11487,9 @@
       <c r="K18" t="s">
         <v>226</v>
       </c>
+      <c r="L18" t="s">
+        <v>309</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
@@ -11449,6 +11525,9 @@
       <c r="K19" t="s">
         <v>226</v>
       </c>
+      <c r="L19" t="s">
+        <v>309</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
@@ -11484,6 +11563,9 @@
       <c r="K20" t="s">
         <v>226</v>
       </c>
+      <c r="L20" t="s">
+        <v>309</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
@@ -11519,6 +11601,9 @@
       <c r="K21" t="s">
         <v>226</v>
       </c>
+      <c r="L21" t="s">
+        <v>309</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
@@ -11554,6 +11639,9 @@
       <c r="K22" t="s">
         <v>230</v>
       </c>
+      <c r="L22" t="s">
+        <v>307</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
@@ -11589,6 +11677,9 @@
       <c r="K23" t="s">
         <v>226</v>
       </c>
+      <c r="L23" t="s">
+        <v>309</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
@@ -11624,6 +11715,9 @@
       <c r="K24" t="s">
         <v>230</v>
       </c>
+      <c r="L24" t="s">
+        <v>307</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
@@ -11659,6 +11753,9 @@
       <c r="K25" t="s">
         <v>226</v>
       </c>
+      <c r="L25" t="s">
+        <v>309</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
@@ -11694,6 +11791,9 @@
       <c r="K26" t="s">
         <v>281</v>
       </c>
+      <c r="L26" t="s">
+        <v>310</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
@@ -11729,6 +11829,9 @@
       <c r="K27" t="s">
         <v>281</v>
       </c>
+      <c r="L27" t="s">
+        <v>310</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
@@ -11764,6 +11867,9 @@
       <c r="K28" t="s">
         <v>281</v>
       </c>
+      <c r="L28" t="s">
+        <v>310</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
@@ -11799,6 +11905,9 @@
       <c r="K29" t="s">
         <v>281</v>
       </c>
+      <c r="L29" t="s">
+        <v>310</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
@@ -11834,6 +11943,9 @@
       <c r="K30" t="s">
         <v>288</v>
       </c>
+      <c r="L30" t="s">
+        <v>311</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
@@ -11869,6 +11981,9 @@
       <c r="K31" t="s">
         <v>288</v>
       </c>
+      <c r="L31" t="s">
+        <v>311</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
@@ -11904,6 +12019,9 @@
       <c r="K32" t="s">
         <v>288</v>
       </c>
+      <c r="L32" t="s">
+        <v>311</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
@@ -11939,6 +12057,9 @@
       <c r="K33" t="s">
         <v>288</v>
       </c>
+      <c r="L33" t="s">
+        <v>311</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
@@ -11974,6 +12095,9 @@
       <c r="K34" t="s">
         <v>288</v>
       </c>
+      <c r="L34" t="s">
+        <v>311</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
@@ -12009,6 +12133,9 @@
       <c r="K35" t="s">
         <v>288</v>
       </c>
+      <c r="L35" t="s">
+        <v>311</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
@@ -12044,6 +12171,9 @@
       <c r="K36" t="s">
         <v>297</v>
       </c>
+      <c r="L36" t="s">
+        <v>312</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
@@ -12079,6 +12209,9 @@
       <c r="K37" t="s">
         <v>297</v>
       </c>
+      <c r="L37" t="s">
+        <v>312</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
@@ -12114,6 +12247,9 @@
       <c r="K38" t="s">
         <v>297</v>
       </c>
+      <c r="L38" t="s">
+        <v>312</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
@@ -12149,6 +12285,9 @@
       <c r="K39" t="s">
         <v>297</v>
       </c>
+      <c r="L39" t="s">
+        <v>312</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
@@ -12184,6 +12323,9 @@
       <c r="K40" t="s">
         <v>297</v>
       </c>
+      <c r="L40" t="s">
+        <v>312</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
@@ -12218,13 +12360,16 @@
       </c>
       <c r="K41" t="s">
         <v>297</v>
+      </c>
+      <c r="L41" t="s">
+        <v>312</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId8"/>
+    <tablePart r:id="rId9"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>